<commit_message>
Soporte para indicadores semestrales, sentido y unidades
- Agregar calcular_cumplimiento con soporte para Sentido (Creciente/Decreciente)
- Nueva funcion obtener_historico_indicador_completo para manejar periodicidad
- Graficos historicos con periodos semestrales (2024-1, 2024-2, etc.)
- Formateo de valores segun unidad (%, $, ENT, Decimales)
- Tabla de datos con periodos y cumplimiento calculado correctamente
- Indicadores decrecientes: menor valor = mejor desempeno

Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/Data/Dataset_Unificado.xlsx
+++ b/Data/Dataset_Unificado.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5f15395a9ed9a48f/Imágenes/Proyectos/Indicadores/Modelo_Prospectivo/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5f15395a9ed9a48f/Proyectos_DS/PDI_2022_2025/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1370" documentId="11_C54DB9D477E07092D1C9E253F65DD242EE9209D1" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AC4E1B31-F2FA-4057-9F79-BA07D36222A5}"/>
+  <xr:revisionPtr revIDLastSave="1371" documentId="11_C54DB9D477E07092D1C9E253F65DD242EE9209D1" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{80F1D9A9-0416-4836-BAC9-CD5BD72E1B69}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1954,8 +1954,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AC494"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="O1" sqref="O1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -43979,6 +43979,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:AC494" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AC480">
     <sortCondition ref="A2:A480"/>
     <sortCondition ref="F2:F480"/>

</xml_diff>

<commit_message>
Actualizar datos del Dataset
Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/Data/Dataset_Unificado.xlsx
+++ b/Data/Dataset_Unificado.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5f15395a9ed9a48f/Proyectos_DS/PDI_2022_2025/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2034" documentId="11_C54DB9D477E07092D1C9E253F65DD242EE9209D1" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CBBF4A51-C18F-4652-9965-8D0331824F8F}"/>
+  <xr:revisionPtr revIDLastSave="2175" documentId="11_C54DB9D477E07092D1C9E253F65DD242EE9209D1" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{47272230-57A3-4A1B-8397-976C1A73F68E}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Base_Indicadores!$A$1:$M$58</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Unificado!$A$1:$AC$503</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Unificado!$A$1:$AC$526</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14244" uniqueCount="518">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14696" uniqueCount="520">
   <si>
     <t>Id</t>
   </si>
@@ -1595,6 +1595,12 @@
   <si>
     <t>369-2025-12-31</t>
   </si>
+  <si>
+    <t>Avance</t>
+  </si>
+  <si>
+    <t>205-2022-12-31</t>
+  </si>
 </sst>
 </file>
 
@@ -1999,9 +2005,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AC503"/>
+  <dimension ref="A1:AC527"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -14033,10 +14041,10 @@
         <v>2</v>
       </c>
       <c r="K140">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="L140">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="M140">
         <v>1</v>
@@ -14119,10 +14127,10 @@
         <v>45</v>
       </c>
       <c r="K141">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="L141">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="M141">
         <v>1</v>
@@ -14803,17 +14811,14 @@
       <c r="I149" t="s">
         <v>465</v>
       </c>
+      <c r="J149">
+        <v>2</v>
+      </c>
       <c r="K149">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="L149">
-        <v>10</v>
-      </c>
-      <c r="M149">
-        <v>1</v>
-      </c>
-      <c r="N149">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O149" t="s">
         <v>35</v>
@@ -14831,7 +14836,7 @@
         <v>0</v>
       </c>
       <c r="T149" t="s">
-        <v>443</v>
+        <v>31</v>
       </c>
       <c r="U149" t="s">
         <v>37</v>
@@ -15318,7 +15323,7 @@
         <v>4.66</v>
       </c>
       <c r="M155">
-        <f>+L155/K155</f>
+        <f>IF(+L155/K155&gt;1.3,1.3,L155/K155)</f>
         <v>0.93200000000000005</v>
       </c>
       <c r="N155">
@@ -15409,8 +15414,8 @@
         <v>3.57</v>
       </c>
       <c r="M156">
-        <f t="shared" ref="M156:M163" si="24">+L156/K156</f>
-        <v>1.4279999999999999</v>
+        <f t="shared" ref="M156:M163" si="24">IF(+L156/K156&gt;1.3,1.3,L156/K156)</f>
+        <v>1.3</v>
       </c>
       <c r="N156">
         <f t="shared" ref="N156:N163" si="25">+L156/K156</f>
@@ -16019,30 +16024,33 @@
         <v>32</v>
       </c>
       <c r="F163" s="3">
-        <v>45838</v>
+        <v>46022</v>
       </c>
       <c r="G163">
         <v>2025</v>
       </c>
       <c r="H163" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="I163" t="s">
-        <v>404</v>
+        <v>465</v>
+      </c>
+      <c r="J163">
+        <v>2</v>
       </c>
       <c r="K163">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="L163">
-        <v>4.08</v>
+        <v>6.78</v>
       </c>
       <c r="M163">
         <f t="shared" si="24"/>
-        <v>1.02</v>
+        <v>1.3</v>
       </c>
       <c r="N163">
-        <f t="shared" si="25"/>
-        <v>1.02</v>
+        <f>+L163/K163</f>
+        <v>1.3560000000000001</v>
       </c>
       <c r="O163" t="s">
         <v>58</v>
@@ -16051,7 +16059,7 @@
         <v>58</v>
       </c>
       <c r="Q163" t="s">
-        <v>406</v>
+        <v>510</v>
       </c>
       <c r="R163">
         <v>0</v>
@@ -16060,7 +16068,7 @@
         <v>1</v>
       </c>
       <c r="T163" t="s">
-        <v>443</v>
+        <v>31</v>
       </c>
       <c r="U163" t="s">
         <v>37</v>
@@ -20705,6 +20713,10 @@
       <c r="I216" t="s">
         <v>465</v>
       </c>
+      <c r="K216">
+        <f>128448131182/1000000</f>
+        <v>128448.131182</v>
+      </c>
       <c r="L216">
         <f>128448131182/1000000</f>
         <v>128448.131182</v>
@@ -20885,7 +20897,7 @@
         <v>143</v>
       </c>
       <c r="Q218" t="s">
-        <v>163</v>
+        <v>519</v>
       </c>
       <c r="R218">
         <v>0</v>
@@ -21569,6 +21581,9 @@
       <c r="I226" t="s">
         <v>465</v>
       </c>
+      <c r="K226">
+        <v>4684</v>
+      </c>
       <c r="L226">
         <v>4684</v>
       </c>
@@ -39253,7 +39268,7 @@
         <v>1</v>
       </c>
       <c r="N429">
-        <f>+L429/K429</f>
+        <f t="shared" ref="N429:N435" si="68">+L429/K429</f>
         <v>1</v>
       </c>
       <c r="O429" t="s">
@@ -39343,7 +39358,7 @@
         <v>1</v>
       </c>
       <c r="N430">
-        <f>+L430/K430</f>
+        <f t="shared" si="68"/>
         <v>1</v>
       </c>
       <c r="O430" t="s">
@@ -39435,7 +39450,7 @@
         <v>1.3</v>
       </c>
       <c r="N431">
-        <f>+L431/K431</f>
+        <f t="shared" si="68"/>
         <v>2.7839074929774967</v>
       </c>
       <c r="O431" t="s">
@@ -39520,11 +39535,11 @@
         <v>3779.9283479999999</v>
       </c>
       <c r="M432">
-        <f t="shared" ref="M432:M435" si="68">IF(+L432/K432&gt;1.3,1.3,L432/K432)</f>
+        <f t="shared" ref="M432:M435" si="69">IF(+L432/K432&gt;1.3,1.3,L432/K432)</f>
         <v>1.3</v>
       </c>
       <c r="N432">
-        <f>+L432/K432</f>
+        <f t="shared" si="68"/>
         <v>2.7839074929774967</v>
       </c>
       <c r="O432" t="s">
@@ -39611,11 +39626,11 @@
         <v>4694.2130900000002</v>
       </c>
       <c r="M433">
+        <f t="shared" si="69"/>
+        <v>1.3</v>
+      </c>
+      <c r="N433">
         <f t="shared" si="68"/>
-        <v>1.3</v>
-      </c>
-      <c r="N433">
-        <f>+L433/K433</f>
         <v>1.3708904125402521</v>
       </c>
       <c r="O433" t="s">
@@ -39699,11 +39714,11 @@
         <v>4694.2130900000002</v>
       </c>
       <c r="M434">
+        <f t="shared" si="69"/>
+        <v>1.3</v>
+      </c>
+      <c r="N434">
         <f t="shared" si="68"/>
-        <v>1.3</v>
-      </c>
-      <c r="N434">
-        <f>+L434/K434</f>
         <v>1.3708904125402521</v>
       </c>
       <c r="O434" t="s">
@@ -39792,11 +39807,11 @@
         <v>3067.3726689999999</v>
       </c>
       <c r="M435">
+        <f t="shared" si="69"/>
+        <v>0.75875626783059102</v>
+      </c>
+      <c r="N435">
         <f t="shared" si="68"/>
-        <v>0.75875626783059102</v>
-      </c>
-      <c r="N435">
-        <f>+L435/K435</f>
         <v>0.75875626783059102</v>
       </c>
       <c r="O435" t="s">
@@ -39975,7 +39990,7 @@
         <v>1</v>
       </c>
       <c r="N437">
-        <f t="shared" ref="N437:N443" si="69">L437/K437</f>
+        <f t="shared" ref="N437:N443" si="70">L437/K437</f>
         <v>1</v>
       </c>
       <c r="O437" t="s">
@@ -40063,11 +40078,11 @@
         <v>9868.4183169999997</v>
       </c>
       <c r="M438">
-        <f t="shared" ref="M438:M443" si="70">L438/K438</f>
+        <f t="shared" ref="M438:M443" si="71">L438/K438</f>
         <v>1.393450174618678</v>
       </c>
       <c r="N438">
-        <f t="shared" si="69"/>
+        <f t="shared" si="70"/>
         <v>1.393450174618678</v>
       </c>
       <c r="O438" t="s">
@@ -40152,11 +40167,11 @@
         <v>9868.4183169999997</v>
       </c>
       <c r="M439">
+        <f t="shared" si="71"/>
+        <v>1.393450174618678</v>
+      </c>
+      <c r="N439">
         <f t="shared" si="70"/>
-        <v>1.393450174618678</v>
-      </c>
-      <c r="N439">
-        <f t="shared" si="69"/>
         <v>1.393450174618678</v>
       </c>
       <c r="O439" t="s">
@@ -40243,11 +40258,11 @@
         <v>4170.686009</v>
       </c>
       <c r="M440">
+        <f t="shared" si="71"/>
+        <v>0.54086603411912804</v>
+      </c>
+      <c r="N440">
         <f t="shared" si="70"/>
-        <v>0.54086603411912804</v>
-      </c>
-      <c r="N440">
-        <f t="shared" si="69"/>
         <v>0.54086603411912804</v>
       </c>
       <c r="O440" t="s">
@@ -40331,11 +40346,11 @@
         <v>4170.686009</v>
       </c>
       <c r="M441">
+        <f t="shared" si="71"/>
+        <v>0.54086603411912804</v>
+      </c>
+      <c r="N441">
         <f t="shared" si="70"/>
-        <v>0.54086603411912804</v>
-      </c>
-      <c r="N441">
-        <f t="shared" si="69"/>
         <v>0.54086603411912804</v>
       </c>
       <c r="O441" t="s">
@@ -40424,11 +40439,11 @@
         <v>7810.0131709999996</v>
       </c>
       <c r="M442">
+        <f t="shared" si="71"/>
+        <v>1.0487700727767424</v>
+      </c>
+      <c r="N442">
         <f t="shared" si="70"/>
-        <v>1.0487700727767424</v>
-      </c>
-      <c r="N442">
-        <f t="shared" si="69"/>
         <v>1.0487700727767424</v>
       </c>
       <c r="O442" t="s">
@@ -40508,11 +40523,11 @@
         <v>7810.0131709999996</v>
       </c>
       <c r="M443">
+        <f t="shared" si="71"/>
+        <v>1.0487700727767424</v>
+      </c>
+      <c r="N443">
         <f t="shared" si="70"/>
-        <v>1.0487700727767424</v>
-      </c>
-      <c r="N443">
-        <f t="shared" si="69"/>
         <v>1.0487700727767424</v>
       </c>
       <c r="O443" t="s">
@@ -40685,11 +40700,11 @@
         <v>3805.6621409999998</v>
       </c>
       <c r="M445">
-        <f t="shared" ref="M445:M451" si="71">IF(L445/K445&gt;1.3,1.3,L445/K445)</f>
+        <f t="shared" ref="M445:M451" si="72">IF(L445/K445&gt;1.3,1.3,L445/K445)</f>
         <v>1</v>
       </c>
       <c r="N445">
-        <f t="shared" ref="N445:N451" si="72">L445/K445</f>
+        <f t="shared" ref="N445:N451" si="73">L445/K445</f>
         <v>1</v>
       </c>
       <c r="O445" t="s">
@@ -40777,11 +40792,11 @@
         <v>4048.733862</v>
       </c>
       <c r="M446">
-        <f t="shared" si="71"/>
+        <f t="shared" si="72"/>
         <v>0.71558444628256934</v>
       </c>
       <c r="N446">
-        <f t="shared" si="72"/>
+        <f t="shared" si="73"/>
         <v>0.71558444628256934</v>
       </c>
       <c r="O446" t="s">
@@ -40866,11 +40881,11 @@
         <v>4048.733862</v>
       </c>
       <c r="M447">
-        <f t="shared" si="71"/>
+        <f t="shared" si="72"/>
         <v>0.71558444628256934</v>
       </c>
       <c r="N447">
-        <f t="shared" si="72"/>
+        <f t="shared" si="73"/>
         <v>0.71558444628256934</v>
       </c>
       <c r="O447" t="s">
@@ -40957,11 +40972,11 @@
         <v>4378.2397499999997</v>
       </c>
       <c r="M448">
-        <f t="shared" si="71"/>
+        <f t="shared" si="72"/>
         <v>1.0013905729387031</v>
       </c>
       <c r="N448">
-        <f t="shared" si="72"/>
+        <f t="shared" si="73"/>
         <v>1.0013905729387031</v>
       </c>
       <c r="O448" t="s">
@@ -41045,11 +41060,11 @@
         <v>4378.2397499999997</v>
       </c>
       <c r="M449">
-        <f t="shared" si="71"/>
+        <f t="shared" si="72"/>
         <v>1.0013905729387031</v>
       </c>
       <c r="N449">
-        <f t="shared" si="72"/>
+        <f t="shared" si="73"/>
         <v>1.0013905729387031</v>
       </c>
       <c r="O449" t="s">
@@ -41138,11 +41153,11 @@
         <v>6478.86355</v>
       </c>
       <c r="M450">
-        <f t="shared" si="71"/>
+        <f t="shared" si="72"/>
         <v>1.1634261619768094</v>
       </c>
       <c r="N450">
-        <f t="shared" si="72"/>
+        <f t="shared" si="73"/>
         <v>1.1634261619768094</v>
       </c>
       <c r="O450" t="s">
@@ -41222,11 +41237,11 @@
         <v>6478.86355</v>
       </c>
       <c r="M451">
-        <f t="shared" si="71"/>
+        <f t="shared" si="72"/>
         <v>1.1634261619768094</v>
       </c>
       <c r="N451">
-        <f t="shared" si="72"/>
+        <f t="shared" si="73"/>
         <v>1.1634261619768094</v>
       </c>
       <c r="O451" t="s">
@@ -41395,11 +41410,11 @@
         <v>7.8</v>
       </c>
       <c r="M453">
-        <f t="shared" ref="M453:M458" si="73">+L453/K453</f>
+        <f t="shared" ref="M453:M458" si="74">+L453/K453</f>
         <v>0.88636363636363624</v>
       </c>
       <c r="N453">
-        <f t="shared" ref="N453:N458" si="74">+L453/K453</f>
+        <f t="shared" ref="N453:N458" si="75">+L453/K453</f>
         <v>0.88636363636363624</v>
       </c>
       <c r="O453" t="s">
@@ -41486,11 +41501,11 @@
         <v>7.9</v>
       </c>
       <c r="M454">
-        <f t="shared" si="73"/>
+        <f t="shared" si="74"/>
         <v>0.94047619047619047</v>
       </c>
       <c r="N454">
-        <f t="shared" si="74"/>
+        <f t="shared" si="75"/>
         <v>0.94047619047619047</v>
       </c>
       <c r="O454" t="s">
@@ -41574,11 +41589,11 @@
         <v>7.9</v>
       </c>
       <c r="M455">
-        <f t="shared" si="73"/>
+        <f t="shared" si="74"/>
         <v>0.94047619047619047</v>
       </c>
       <c r="N455">
-        <f t="shared" si="74"/>
+        <f t="shared" si="75"/>
         <v>0.94047619047619047</v>
       </c>
       <c r="O455" t="s">
@@ -41665,11 +41680,11 @@
         <v>12.4</v>
       </c>
       <c r="M456">
-        <f t="shared" si="73"/>
+        <f t="shared" si="74"/>
         <v>1.4939759036144578</v>
       </c>
       <c r="N456">
-        <f t="shared" si="74"/>
+        <f t="shared" si="75"/>
         <v>1.4939759036144578</v>
       </c>
       <c r="O456" t="s">
@@ -41753,11 +41768,11 @@
         <v>12.4</v>
       </c>
       <c r="M457">
-        <f t="shared" si="73"/>
+        <f t="shared" si="74"/>
         <v>1.4939759036144578</v>
       </c>
       <c r="N457">
-        <f t="shared" si="74"/>
+        <f t="shared" si="75"/>
         <v>1.4939759036144578</v>
       </c>
       <c r="O457" t="s">
@@ -41844,11 +41859,11 @@
         <v>15.1</v>
       </c>
       <c r="M458">
-        <f t="shared" si="73"/>
+        <f t="shared" si="74"/>
         <v>1.2583333333333333</v>
       </c>
       <c r="N458">
-        <f t="shared" si="74"/>
+        <f t="shared" si="75"/>
         <v>1.2583333333333333</v>
       </c>
       <c r="O458" t="s">
@@ -42023,11 +42038,11 @@
         <v>5</v>
       </c>
       <c r="M460">
-        <f t="shared" ref="M460:M465" si="75">+L460/K460</f>
+        <f t="shared" ref="M460:M465" si="76">+L460/K460</f>
         <v>0.76923076923076927</v>
       </c>
       <c r="N460">
-        <f t="shared" ref="N460:N465" si="76">+L460/K460</f>
+        <f t="shared" ref="N460:N465" si="77">+L460/K460</f>
         <v>0.76923076923076927</v>
       </c>
       <c r="O460" t="s">
@@ -42114,11 +42129,11 @@
         <v>6</v>
       </c>
       <c r="M461">
-        <f t="shared" si="75"/>
+        <f t="shared" si="76"/>
         <v>1</v>
       </c>
       <c r="N461">
-        <f t="shared" si="76"/>
+        <f t="shared" si="77"/>
         <v>1</v>
       </c>
       <c r="O461" t="s">
@@ -42202,11 +42217,11 @@
         <v>6</v>
       </c>
       <c r="M462">
-        <f t="shared" si="75"/>
+        <f t="shared" si="76"/>
         <v>1</v>
       </c>
       <c r="N462">
-        <f t="shared" si="76"/>
+        <f t="shared" si="77"/>
         <v>1</v>
       </c>
       <c r="O462" t="s">
@@ -42293,11 +42308,11 @@
         <v>9</v>
       </c>
       <c r="M463">
-        <f t="shared" si="75"/>
+        <f t="shared" si="76"/>
         <v>1.2857142857142858</v>
       </c>
       <c r="N463">
-        <f t="shared" si="76"/>
+        <f t="shared" si="77"/>
         <v>1.2857142857142858</v>
       </c>
       <c r="O463" t="s">
@@ -42381,11 +42396,11 @@
         <v>9</v>
       </c>
       <c r="M464">
-        <f t="shared" si="75"/>
+        <f t="shared" si="76"/>
         <v>1.2857142857142858</v>
       </c>
       <c r="N464">
-        <f t="shared" si="76"/>
+        <f t="shared" si="77"/>
         <v>1.2857142857142858</v>
       </c>
       <c r="O464" t="s">
@@ -42472,11 +42487,11 @@
         <v>11</v>
       </c>
       <c r="M465">
-        <f t="shared" si="75"/>
+        <f t="shared" si="76"/>
         <v>1.2222222222222223</v>
       </c>
       <c r="N465">
-        <f t="shared" si="76"/>
+        <f t="shared" si="77"/>
         <v>1.2222222222222223</v>
       </c>
       <c r="O465" t="s">
@@ -43074,7 +43089,7 @@
         <v>1.3</v>
       </c>
       <c r="N472">
-        <f t="shared" ref="N472:N477" si="77">+L472/K472</f>
+        <f t="shared" ref="N472:N477" si="78">+L472/K472</f>
         <v>1.7424000000000002</v>
       </c>
       <c r="O472" t="s">
@@ -43164,7 +43179,7 @@
         <v>1.27</v>
       </c>
       <c r="N473">
-        <f t="shared" si="77"/>
+        <f t="shared" si="78"/>
         <v>1.27</v>
       </c>
       <c r="O473" t="s">
@@ -43251,7 +43266,7 @@
         <v>1.27</v>
       </c>
       <c r="N474">
-        <f t="shared" si="77"/>
+        <f t="shared" si="78"/>
         <v>1.27</v>
       </c>
       <c r="O474" t="s">
@@ -43341,7 +43356,7 @@
         <v>1.0760000000000001</v>
       </c>
       <c r="N475">
-        <f t="shared" si="77"/>
+        <f t="shared" si="78"/>
         <v>1.0759999999999998</v>
       </c>
       <c r="O475" t="s">
@@ -43428,7 +43443,7 @@
         <v>1.0760000000000001</v>
       </c>
       <c r="N476">
-        <f t="shared" si="77"/>
+        <f t="shared" si="78"/>
         <v>1.0759999999999998</v>
       </c>
       <c r="O476" t="s">
@@ -43515,11 +43530,11 @@
         <v>58.6</v>
       </c>
       <c r="M477">
-        <f t="shared" ref="M477:M482" si="78">+L477/K477</f>
+        <f t="shared" ref="M477:M482" si="79">+L477/K477</f>
         <v>1.0654545454545454</v>
       </c>
       <c r="N477">
-        <f t="shared" si="77"/>
+        <f t="shared" si="78"/>
         <v>1.0654545454545454</v>
       </c>
       <c r="O477" t="s">
@@ -43610,11 +43625,11 @@
         <v>165190.90430007299</v>
       </c>
       <c r="M478">
-        <f t="shared" si="78"/>
+        <f t="shared" si="79"/>
         <v>1.0366289952280319</v>
       </c>
       <c r="N478">
-        <f t="shared" ref="N478:N479" si="79">+L478/K478</f>
+        <f t="shared" ref="N478:N479" si="80">+L478/K478</f>
         <v>1.0366289952280319</v>
       </c>
       <c r="O478" t="s">
@@ -43704,11 +43719,11 @@
         <v>332786.049596973</v>
       </c>
       <c r="M479">
-        <f t="shared" si="78"/>
+        <f t="shared" si="79"/>
         <v>1.0759165719522106</v>
       </c>
       <c r="N479">
-        <f t="shared" si="79"/>
+        <f t="shared" si="80"/>
         <v>1.0759165719522106</v>
       </c>
       <c r="O479" t="s">
@@ -43796,8 +43811,8 @@
         <v>6.78</v>
       </c>
       <c r="M480">
-        <f t="shared" si="78"/>
-        <v>1.3560000000000001</v>
+        <f>IF(+L480/K480&gt;1.3,1.3,L480/K480)</f>
+        <v>1.3</v>
       </c>
       <c r="N480">
         <f>+L480/K480</f>
@@ -43819,7 +43834,7 @@
         <v>1</v>
       </c>
       <c r="T480" t="s">
-        <v>31</v>
+        <v>443</v>
       </c>
       <c r="U480" t="s">
         <v>37</v>
@@ -43884,7 +43899,7 @@
         <v>58.6</v>
       </c>
       <c r="M481">
-        <f t="shared" si="78"/>
+        <f t="shared" si="79"/>
         <v>1.0654545454545454</v>
       </c>
       <c r="N481">
@@ -43975,7 +43990,7 @@
         <v>94</v>
       </c>
       <c r="M482">
-        <f t="shared" si="78"/>
+        <f t="shared" si="79"/>
         <v>1.175</v>
       </c>
       <c r="N482">
@@ -45097,11 +45112,11 @@
         <v>89.9</v>
       </c>
       <c r="M495">
-        <f t="shared" ref="M495" si="80">+L495/K495</f>
+        <f t="shared" ref="M495" si="81">+L495/K495</f>
         <v>1.0576470588235294</v>
       </c>
       <c r="N495">
-        <f t="shared" ref="N495" si="81">+L495/K495</f>
+        <f t="shared" ref="N495" si="82">+L495/K495</f>
         <v>1.0576470588235294</v>
       </c>
       <c r="O495" t="s">
@@ -45358,9 +45373,6 @@
       <c r="I498" t="s">
         <v>465</v>
       </c>
-      <c r="J498">
-        <v>2</v>
-      </c>
       <c r="K498">
         <v>86.1</v>
       </c>
@@ -45368,11 +45380,11 @@
         <v>86.2</v>
       </c>
       <c r="M498">
-        <f t="shared" ref="M498" si="82">+L498/K498</f>
+        <f t="shared" ref="M498" si="83">+L498/K498</f>
         <v>1.0011614401858304</v>
       </c>
       <c r="N498">
-        <f t="shared" ref="N498" si="83">+L498/K498</f>
+        <f t="shared" ref="N498" si="84">+L498/K498</f>
         <v>1.0011614401858304</v>
       </c>
       <c r="O498" t="s">
@@ -45456,11 +45468,11 @@
         <v>82.81</v>
       </c>
       <c r="M499">
-        <f t="shared" ref="M499:M500" si="84">+K499/L499</f>
+        <f t="shared" ref="M499:M500" si="85">+K499/L499</f>
         <v>0.97814273638449456</v>
       </c>
       <c r="N499">
-        <f t="shared" ref="N499:N500" si="85">+K499/L499</f>
+        <f t="shared" ref="N499:N500" si="86">+K499/L499</f>
         <v>0.97814273638449456</v>
       </c>
       <c r="O499" t="s">
@@ -45544,11 +45556,11 @@
         <v>68.400000000000006</v>
       </c>
       <c r="M500">
-        <f t="shared" si="84"/>
+        <f t="shared" si="85"/>
         <v>1.0380116959064327</v>
       </c>
       <c r="N500">
-        <f t="shared" si="85"/>
+        <f t="shared" si="86"/>
         <v>1.0380116959064327</v>
       </c>
       <c r="O500" t="s">
@@ -45632,11 +45644,11 @@
         <v>70233</v>
       </c>
       <c r="M501">
-        <f t="shared" ref="M501:M502" si="86">+L501/K501</f>
+        <f t="shared" ref="M501:M502" si="87">+L501/K501</f>
         <v>0.84417707369256101</v>
       </c>
       <c r="N501">
-        <f t="shared" ref="N501" si="87">+L501/K501</f>
+        <f t="shared" ref="N501" si="88">+L501/K501</f>
         <v>0.84417707369256101</v>
       </c>
       <c r="O501" t="s">
@@ -45720,7 +45732,7 @@
         <v>190</v>
       </c>
       <c r="M502">
-        <f t="shared" si="86"/>
+        <f t="shared" si="87"/>
         <v>1</v>
       </c>
       <c r="N502">
@@ -45862,6 +45874,2106 @@
       </c>
       <c r="AC503" t="s">
         <v>31</v>
+      </c>
+    </row>
+    <row r="504" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A504">
+        <v>14</v>
+      </c>
+      <c r="B504" t="s">
+        <v>29</v>
+      </c>
+      <c r="C504" t="s">
+        <v>186</v>
+      </c>
+      <c r="D504" t="s">
+        <v>31</v>
+      </c>
+      <c r="E504" t="s">
+        <v>32</v>
+      </c>
+      <c r="F504" s="3">
+        <v>46023</v>
+      </c>
+      <c r="G504">
+        <v>2026</v>
+      </c>
+      <c r="H504" t="s">
+        <v>518</v>
+      </c>
+      <c r="I504" t="s">
+        <v>518</v>
+      </c>
+      <c r="K504">
+        <v>55756</v>
+      </c>
+      <c r="L504" s="4">
+        <v>56931</v>
+      </c>
+      <c r="M504">
+        <f>+L504/K504</f>
+        <v>1.0210739651337972</v>
+      </c>
+      <c r="N504">
+        <f>+L504/K504</f>
+        <v>1.0210739651337972</v>
+      </c>
+      <c r="O504" t="s">
+        <v>35</v>
+      </c>
+      <c r="P504" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q504" t="s">
+        <v>481</v>
+      </c>
+      <c r="R504">
+        <v>0</v>
+      </c>
+      <c r="S504">
+        <v>0</v>
+      </c>
+      <c r="T504" t="s">
+        <v>518</v>
+      </c>
+      <c r="U504" t="s">
+        <v>37</v>
+      </c>
+      <c r="V504" t="s">
+        <v>30</v>
+      </c>
+      <c r="W504" t="s">
+        <v>38</v>
+      </c>
+      <c r="X504" t="s">
+        <v>39</v>
+      </c>
+      <c r="Y504" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z504" t="s">
+        <v>41</v>
+      </c>
+      <c r="AA504" t="s">
+        <v>42</v>
+      </c>
+      <c r="AB504" t="s">
+        <v>43</v>
+      </c>
+      <c r="AC504" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="505" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A505">
+        <v>14.1</v>
+      </c>
+      <c r="B505" t="s">
+        <v>353</v>
+      </c>
+      <c r="C505" t="s">
+        <v>186</v>
+      </c>
+      <c r="D505" t="s">
+        <v>31</v>
+      </c>
+      <c r="E505" t="s">
+        <v>32</v>
+      </c>
+      <c r="F505" s="3">
+        <v>46023</v>
+      </c>
+      <c r="G505">
+        <v>2026</v>
+      </c>
+      <c r="H505" t="s">
+        <v>518</v>
+      </c>
+      <c r="I505" t="s">
+        <v>518</v>
+      </c>
+      <c r="K505">
+        <v>16981</v>
+      </c>
+      <c r="L505">
+        <v>17472</v>
+      </c>
+      <c r="M505">
+        <f>+L505/K505</f>
+        <v>1.0289146693363171</v>
+      </c>
+      <c r="N505">
+        <f>+L505/K505</f>
+        <v>1.0289146693363171</v>
+      </c>
+      <c r="O505" t="s">
+        <v>35</v>
+      </c>
+      <c r="P505" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q505" t="s">
+        <v>482</v>
+      </c>
+      <c r="R505">
+        <v>0</v>
+      </c>
+      <c r="S505">
+        <v>0</v>
+      </c>
+      <c r="T505" t="s">
+        <v>518</v>
+      </c>
+      <c r="U505" t="s">
+        <v>37</v>
+      </c>
+      <c r="V505" t="s">
+        <v>30</v>
+      </c>
+      <c r="W505" t="s">
+        <v>38</v>
+      </c>
+      <c r="X505" t="s">
+        <v>39</v>
+      </c>
+      <c r="Y505" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z505" t="s">
+        <v>86</v>
+      </c>
+      <c r="AA505" t="s">
+        <v>339</v>
+      </c>
+      <c r="AB505" t="s">
+        <v>78</v>
+      </c>
+      <c r="AC505" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="506" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A506">
+        <v>14.2</v>
+      </c>
+      <c r="B506" t="s">
+        <v>359</v>
+      </c>
+      <c r="C506" t="s">
+        <v>186</v>
+      </c>
+      <c r="D506" t="s">
+        <v>31</v>
+      </c>
+      <c r="E506" t="s">
+        <v>32</v>
+      </c>
+      <c r="F506" s="3">
+        <v>46023</v>
+      </c>
+      <c r="G506">
+        <v>2026</v>
+      </c>
+      <c r="H506" t="s">
+        <v>518</v>
+      </c>
+      <c r="I506" t="s">
+        <v>518</v>
+      </c>
+      <c r="K506">
+        <v>92409</v>
+      </c>
+      <c r="L506">
+        <v>95964</v>
+      </c>
+      <c r="M506">
+        <f>+L506/K506</f>
+        <v>1.0384702788689413</v>
+      </c>
+      <c r="N506">
+        <f>+L506/K506</f>
+        <v>1.0384702788689413</v>
+      </c>
+      <c r="O506" t="s">
+        <v>35</v>
+      </c>
+      <c r="P506" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q506" t="s">
+        <v>415</v>
+      </c>
+      <c r="R506">
+        <v>0</v>
+      </c>
+      <c r="S506">
+        <v>0</v>
+      </c>
+      <c r="T506" t="s">
+        <v>518</v>
+      </c>
+      <c r="U506" t="s">
+        <v>37</v>
+      </c>
+      <c r="V506" t="s">
+        <v>30</v>
+      </c>
+      <c r="W506" t="s">
+        <v>38</v>
+      </c>
+      <c r="X506" t="s">
+        <v>39</v>
+      </c>
+      <c r="Y506" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z506" t="s">
+        <v>86</v>
+      </c>
+      <c r="AA506" t="s">
+        <v>339</v>
+      </c>
+      <c r="AB506" t="s">
+        <v>78</v>
+      </c>
+      <c r="AC506" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="507" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A507">
+        <v>14.3</v>
+      </c>
+      <c r="B507" t="s">
+        <v>365</v>
+      </c>
+      <c r="C507" t="s">
+        <v>186</v>
+      </c>
+      <c r="D507" t="s">
+        <v>31</v>
+      </c>
+      <c r="E507" t="s">
+        <v>32</v>
+      </c>
+      <c r="F507" s="3">
+        <v>46023</v>
+      </c>
+      <c r="G507">
+        <v>2026</v>
+      </c>
+      <c r="H507" t="s">
+        <v>518</v>
+      </c>
+      <c r="I507" t="s">
+        <v>518</v>
+      </c>
+      <c r="K507">
+        <v>101379</v>
+      </c>
+      <c r="L507">
+        <v>104367</v>
+      </c>
+      <c r="M507">
+        <f t="shared" ref="M507:M508" si="89">+L507/K507</f>
+        <v>1.0294735596129376</v>
+      </c>
+      <c r="N507">
+        <f t="shared" ref="N507:N508" si="90">+L507/K507</f>
+        <v>1.0294735596129376</v>
+      </c>
+      <c r="O507" t="s">
+        <v>35</v>
+      </c>
+      <c r="P507" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q507" t="s">
+        <v>484</v>
+      </c>
+      <c r="R507">
+        <v>0</v>
+      </c>
+      <c r="S507">
+        <v>0</v>
+      </c>
+      <c r="T507" t="s">
+        <v>518</v>
+      </c>
+      <c r="U507" t="s">
+        <v>37</v>
+      </c>
+      <c r="V507" t="s">
+        <v>30</v>
+      </c>
+      <c r="W507" t="s">
+        <v>38</v>
+      </c>
+      <c r="X507" t="s">
+        <v>39</v>
+      </c>
+      <c r="Y507" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z507" t="s">
+        <v>86</v>
+      </c>
+      <c r="AA507" t="s">
+        <v>339</v>
+      </c>
+      <c r="AB507" t="s">
+        <v>78</v>
+      </c>
+      <c r="AC507" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="508" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A508">
+        <v>14.4</v>
+      </c>
+      <c r="B508" t="s">
+        <v>371</v>
+      </c>
+      <c r="C508" t="s">
+        <v>186</v>
+      </c>
+      <c r="D508" t="s">
+        <v>31</v>
+      </c>
+      <c r="E508" t="s">
+        <v>32</v>
+      </c>
+      <c r="F508" s="3">
+        <v>46023</v>
+      </c>
+      <c r="G508">
+        <v>2026</v>
+      </c>
+      <c r="H508" t="s">
+        <v>518</v>
+      </c>
+      <c r="I508" t="s">
+        <v>518</v>
+      </c>
+      <c r="K508">
+        <f>+K506+K507</f>
+        <v>193788</v>
+      </c>
+      <c r="L508">
+        <f>+L506+L507</f>
+        <v>200331</v>
+      </c>
+      <c r="M508">
+        <f t="shared" si="89"/>
+        <v>1.033763700538733</v>
+      </c>
+      <c r="N508">
+        <f t="shared" si="90"/>
+        <v>1.033763700538733</v>
+      </c>
+      <c r="O508" t="s">
+        <v>35</v>
+      </c>
+      <c r="P508" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q508" t="s">
+        <v>485</v>
+      </c>
+      <c r="R508">
+        <v>0</v>
+      </c>
+      <c r="S508">
+        <v>0</v>
+      </c>
+      <c r="T508" t="s">
+        <v>518</v>
+      </c>
+      <c r="U508" t="s">
+        <v>37</v>
+      </c>
+      <c r="V508" t="s">
+        <v>30</v>
+      </c>
+      <c r="W508" t="s">
+        <v>38</v>
+      </c>
+      <c r="X508" t="s">
+        <v>39</v>
+      </c>
+      <c r="Y508" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z508" t="s">
+        <v>86</v>
+      </c>
+      <c r="AA508" t="s">
+        <v>339</v>
+      </c>
+      <c r="AB508" t="s">
+        <v>78</v>
+      </c>
+      <c r="AC508" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="509" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A509">
+        <v>77</v>
+      </c>
+      <c r="B509" t="s">
+        <v>55</v>
+      </c>
+      <c r="C509" t="s">
+        <v>56</v>
+      </c>
+      <c r="D509" t="s">
+        <v>57</v>
+      </c>
+      <c r="E509" t="s">
+        <v>32</v>
+      </c>
+      <c r="F509" s="3">
+        <v>46023</v>
+      </c>
+      <c r="G509">
+        <v>2026</v>
+      </c>
+      <c r="H509" t="s">
+        <v>518</v>
+      </c>
+      <c r="I509" t="s">
+        <v>518</v>
+      </c>
+      <c r="K509">
+        <v>97</v>
+      </c>
+      <c r="L509">
+        <v>97.17</v>
+      </c>
+      <c r="M509">
+        <f>+L509/K509</f>
+        <v>1.0017525773195877</v>
+      </c>
+      <c r="N509">
+        <f>+L509/K509</f>
+        <v>1.0017525773195877</v>
+      </c>
+      <c r="O509" t="s">
+        <v>58</v>
+      </c>
+      <c r="P509" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q509" t="s">
+        <v>503</v>
+      </c>
+      <c r="R509">
+        <v>0</v>
+      </c>
+      <c r="S509">
+        <v>1</v>
+      </c>
+      <c r="T509" t="s">
+        <v>518</v>
+      </c>
+      <c r="U509" t="s">
+        <v>37</v>
+      </c>
+      <c r="V509" t="s">
+        <v>56</v>
+      </c>
+      <c r="W509" t="s">
+        <v>60</v>
+      </c>
+      <c r="X509" t="s">
+        <v>61</v>
+      </c>
+      <c r="Y509" t="s">
+        <v>62</v>
+      </c>
+      <c r="Z509" t="s">
+        <v>63</v>
+      </c>
+      <c r="AA509" t="s">
+        <v>64</v>
+      </c>
+      <c r="AB509" t="s">
+        <v>65</v>
+      </c>
+      <c r="AC509" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="510" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A510">
+        <v>96</v>
+      </c>
+      <c r="B510" t="s">
+        <v>70</v>
+      </c>
+      <c r="C510" t="s">
+        <v>71</v>
+      </c>
+      <c r="D510" t="s">
+        <v>66</v>
+      </c>
+      <c r="E510" t="s">
+        <v>32</v>
+      </c>
+      <c r="F510" s="3">
+        <v>46023</v>
+      </c>
+      <c r="G510">
+        <v>2026</v>
+      </c>
+      <c r="H510" t="s">
+        <v>518</v>
+      </c>
+      <c r="I510" t="s">
+        <v>518</v>
+      </c>
+      <c r="K510">
+        <v>2531</v>
+      </c>
+      <c r="L510">
+        <v>2169</v>
+      </c>
+      <c r="M510">
+        <f>+L510/K510</f>
+        <v>0.85697352824970363</v>
+      </c>
+      <c r="N510">
+        <f>+L510/K510</f>
+        <v>0.85697352824970363</v>
+      </c>
+      <c r="O510" t="s">
+        <v>35</v>
+      </c>
+      <c r="P510" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q510" t="s">
+        <v>507</v>
+      </c>
+      <c r="R510">
+        <v>0</v>
+      </c>
+      <c r="S510">
+        <v>0</v>
+      </c>
+      <c r="T510" t="s">
+        <v>518</v>
+      </c>
+      <c r="U510" t="s">
+        <v>37</v>
+      </c>
+      <c r="V510" t="s">
+        <v>71</v>
+      </c>
+      <c r="W510" t="s">
+        <v>73</v>
+      </c>
+      <c r="X510" t="s">
+        <v>74</v>
+      </c>
+      <c r="Y510" t="s">
+        <v>75</v>
+      </c>
+      <c r="Z510" t="s">
+        <v>76</v>
+      </c>
+      <c r="AA510" t="s">
+        <v>77</v>
+      </c>
+      <c r="AB510" t="s">
+        <v>78</v>
+      </c>
+      <c r="AC510" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="511" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A511">
+        <v>98</v>
+      </c>
+      <c r="B511" t="s">
+        <v>91</v>
+      </c>
+      <c r="C511" t="s">
+        <v>83</v>
+      </c>
+      <c r="D511" t="s">
+        <v>31</v>
+      </c>
+      <c r="E511" t="s">
+        <v>32</v>
+      </c>
+      <c r="F511" s="3">
+        <v>46022</v>
+      </c>
+      <c r="G511">
+        <v>2025</v>
+      </c>
+      <c r="H511" t="s">
+        <v>44</v>
+      </c>
+      <c r="I511" t="s">
+        <v>465</v>
+      </c>
+      <c r="K511">
+        <v>10</v>
+      </c>
+      <c r="L511">
+        <v>10</v>
+      </c>
+      <c r="M511">
+        <v>1</v>
+      </c>
+      <c r="N511">
+        <v>1</v>
+      </c>
+      <c r="O511" t="s">
+        <v>35</v>
+      </c>
+      <c r="P511" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q511" t="s">
+        <v>509</v>
+      </c>
+      <c r="R511">
+        <v>0</v>
+      </c>
+      <c r="S511">
+        <v>0</v>
+      </c>
+      <c r="T511" t="s">
+        <v>443</v>
+      </c>
+      <c r="U511" t="s">
+        <v>37</v>
+      </c>
+      <c r="V511" t="s">
+        <v>83</v>
+      </c>
+      <c r="W511" t="s">
+        <v>38</v>
+      </c>
+      <c r="X511" t="s">
+        <v>39</v>
+      </c>
+      <c r="Y511" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z511" t="s">
+        <v>86</v>
+      </c>
+      <c r="AA511" t="s">
+        <v>87</v>
+      </c>
+      <c r="AB511" t="s">
+        <v>78</v>
+      </c>
+      <c r="AC511" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="512" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A512">
+        <v>98</v>
+      </c>
+      <c r="B512" t="s">
+        <v>91</v>
+      </c>
+      <c r="C512" t="s">
+        <v>83</v>
+      </c>
+      <c r="D512" t="s">
+        <v>31</v>
+      </c>
+      <c r="E512" t="s">
+        <v>32</v>
+      </c>
+      <c r="F512" s="3">
+        <v>46023</v>
+      </c>
+      <c r="G512">
+        <v>2026</v>
+      </c>
+      <c r="H512" t="s">
+        <v>518</v>
+      </c>
+      <c r="I512" t="s">
+        <v>518</v>
+      </c>
+      <c r="K512">
+        <f>+K141+K144+K147+K511</f>
+        <v>20</v>
+      </c>
+      <c r="L512">
+        <f>+L141+L144+L147+L511</f>
+        <v>20</v>
+      </c>
+      <c r="M512">
+        <v>1</v>
+      </c>
+      <c r="N512">
+        <v>1</v>
+      </c>
+      <c r="O512" t="s">
+        <v>35</v>
+      </c>
+      <c r="P512" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q512" t="s">
+        <v>509</v>
+      </c>
+      <c r="R512">
+        <v>0</v>
+      </c>
+      <c r="S512">
+        <v>0</v>
+      </c>
+      <c r="T512" t="s">
+        <v>518</v>
+      </c>
+      <c r="U512" t="s">
+        <v>37</v>
+      </c>
+      <c r="V512" t="s">
+        <v>83</v>
+      </c>
+      <c r="W512" t="s">
+        <v>38</v>
+      </c>
+      <c r="X512" t="s">
+        <v>39</v>
+      </c>
+      <c r="Y512" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z512" t="s">
+        <v>86</v>
+      </c>
+      <c r="AA512" t="s">
+        <v>87</v>
+      </c>
+      <c r="AB512" t="s">
+        <v>78</v>
+      </c>
+      <c r="AC512" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="513" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A513">
+        <v>109</v>
+      </c>
+      <c r="B513" t="s">
+        <v>96</v>
+      </c>
+      <c r="C513" t="s">
+        <v>99</v>
+      </c>
+      <c r="D513" t="s">
+        <v>66</v>
+      </c>
+      <c r="E513" t="s">
+        <v>32</v>
+      </c>
+      <c r="F513" s="3">
+        <v>46023</v>
+      </c>
+      <c r="G513">
+        <v>2026</v>
+      </c>
+      <c r="H513" t="s">
+        <v>518</v>
+      </c>
+      <c r="I513" t="s">
+        <v>518</v>
+      </c>
+      <c r="K513">
+        <v>80</v>
+      </c>
+      <c r="L513">
+        <v>94</v>
+      </c>
+      <c r="M513">
+        <f t="shared" ref="M513:M514" si="91">+L513/K513</f>
+        <v>1.175</v>
+      </c>
+      <c r="N513">
+        <v>1.0625</v>
+      </c>
+      <c r="O513" t="s">
+        <v>58</v>
+      </c>
+      <c r="P513" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q513" t="s">
+        <v>488</v>
+      </c>
+      <c r="R513">
+        <v>0</v>
+      </c>
+      <c r="S513">
+        <v>0</v>
+      </c>
+      <c r="T513" t="s">
+        <v>518</v>
+      </c>
+      <c r="U513" t="s">
+        <v>37</v>
+      </c>
+      <c r="V513" t="s">
+        <v>99</v>
+      </c>
+      <c r="W513" t="s">
+        <v>60</v>
+      </c>
+      <c r="X513" t="s">
+        <v>100</v>
+      </c>
+      <c r="Z513" t="s">
+        <v>101</v>
+      </c>
+      <c r="AA513" t="s">
+        <v>102</v>
+      </c>
+      <c r="AB513" t="s">
+        <v>65</v>
+      </c>
+      <c r="AC513" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="514" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A514">
+        <v>148</v>
+      </c>
+      <c r="B514" t="s">
+        <v>104</v>
+      </c>
+      <c r="C514" t="s">
+        <v>105</v>
+      </c>
+      <c r="D514" t="s">
+        <v>31</v>
+      </c>
+      <c r="E514" t="s">
+        <v>32</v>
+      </c>
+      <c r="F514" s="3">
+        <v>46023</v>
+      </c>
+      <c r="G514">
+        <v>2026</v>
+      </c>
+      <c r="H514" t="s">
+        <v>518</v>
+      </c>
+      <c r="I514" t="s">
+        <v>518</v>
+      </c>
+      <c r="J514">
+        <v>2</v>
+      </c>
+      <c r="K514">
+        <v>5</v>
+      </c>
+      <c r="L514">
+        <v>5.8624999999999998</v>
+      </c>
+      <c r="M514">
+        <f>IF(+L514/K514&gt;1.3,1.3,L514/K514)</f>
+        <v>1.1724999999999999</v>
+      </c>
+      <c r="N514">
+        <f>+L514/K514</f>
+        <v>1.1724999999999999</v>
+      </c>
+      <c r="O514" t="s">
+        <v>58</v>
+      </c>
+      <c r="P514" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q514" t="s">
+        <v>510</v>
+      </c>
+      <c r="R514">
+        <v>0</v>
+      </c>
+      <c r="S514">
+        <v>1</v>
+      </c>
+      <c r="T514" t="s">
+        <v>518</v>
+      </c>
+      <c r="U514" t="s">
+        <v>37</v>
+      </c>
+      <c r="V514" t="s">
+        <v>105</v>
+      </c>
+      <c r="W514" t="s">
+        <v>73</v>
+      </c>
+      <c r="X514" t="s">
+        <v>74</v>
+      </c>
+      <c r="Y514" t="s">
+        <v>75</v>
+      </c>
+      <c r="Z514" t="s">
+        <v>76</v>
+      </c>
+      <c r="AA514" t="s">
+        <v>77</v>
+      </c>
+      <c r="AB514" t="s">
+        <v>43</v>
+      </c>
+      <c r="AC514" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="515" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A515">
+        <v>193</v>
+      </c>
+      <c r="B515" s="5" t="s">
+        <v>478</v>
+      </c>
+      <c r="C515" t="s">
+        <v>30</v>
+      </c>
+      <c r="D515" t="s">
+        <v>31</v>
+      </c>
+      <c r="E515" t="s">
+        <v>32</v>
+      </c>
+      <c r="F515" s="3">
+        <v>46023</v>
+      </c>
+      <c r="G515">
+        <v>2026</v>
+      </c>
+      <c r="H515" t="s">
+        <v>518</v>
+      </c>
+      <c r="I515" t="s">
+        <v>518</v>
+      </c>
+      <c r="K515">
+        <v>94</v>
+      </c>
+      <c r="L515">
+        <v>95</v>
+      </c>
+      <c r="M515">
+        <f>+L515/K515</f>
+        <v>1.0106382978723405</v>
+      </c>
+      <c r="N515">
+        <f>+L515/K515</f>
+        <v>1.0106382978723405</v>
+      </c>
+      <c r="O515" t="s">
+        <v>58</v>
+      </c>
+      <c r="P515" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q515" t="s">
+        <v>511</v>
+      </c>
+      <c r="R515">
+        <v>1</v>
+      </c>
+      <c r="S515">
+        <v>1</v>
+      </c>
+      <c r="T515" t="s">
+        <v>518</v>
+      </c>
+      <c r="U515" t="s">
+        <v>37</v>
+      </c>
+      <c r="V515" t="s">
+        <v>30</v>
+      </c>
+      <c r="W515" t="s">
+        <v>112</v>
+      </c>
+      <c r="X515" t="s">
+        <v>113</v>
+      </c>
+      <c r="Y515" t="s">
+        <v>114</v>
+      </c>
+      <c r="Z515" t="s">
+        <v>63</v>
+      </c>
+      <c r="AA515" t="s">
+        <v>115</v>
+      </c>
+      <c r="AB515" t="s">
+        <v>65</v>
+      </c>
+      <c r="AC515" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="516" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A516">
+        <v>194</v>
+      </c>
+      <c r="B516" t="s">
+        <v>121</v>
+      </c>
+      <c r="C516" t="s">
+        <v>30</v>
+      </c>
+      <c r="D516" t="s">
+        <v>31</v>
+      </c>
+      <c r="E516" t="s">
+        <v>32</v>
+      </c>
+      <c r="F516" s="3">
+        <v>46023</v>
+      </c>
+      <c r="G516">
+        <v>2026</v>
+      </c>
+      <c r="H516" t="s">
+        <v>518</v>
+      </c>
+      <c r="I516" t="s">
+        <v>518</v>
+      </c>
+      <c r="K516">
+        <v>85</v>
+      </c>
+      <c r="L516">
+        <v>89.9</v>
+      </c>
+      <c r="M516">
+        <f t="shared" ref="M516" si="92">+L516/K516</f>
+        <v>1.0576470588235294</v>
+      </c>
+      <c r="N516">
+        <f t="shared" ref="N516" si="93">+L516/K516</f>
+        <v>1.0576470588235294</v>
+      </c>
+      <c r="O516" t="s">
+        <v>58</v>
+      </c>
+      <c r="P516" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q516" t="s">
+        <v>419</v>
+      </c>
+      <c r="R516">
+        <v>0</v>
+      </c>
+      <c r="S516">
+        <v>0</v>
+      </c>
+      <c r="T516" t="s">
+        <v>518</v>
+      </c>
+      <c r="U516" t="s">
+        <v>37</v>
+      </c>
+      <c r="V516" t="s">
+        <v>30</v>
+      </c>
+      <c r="W516" t="s">
+        <v>112</v>
+      </c>
+      <c r="X516" t="s">
+        <v>113</v>
+      </c>
+      <c r="Y516" t="s">
+        <v>123</v>
+      </c>
+      <c r="Z516" t="s">
+        <v>41</v>
+      </c>
+      <c r="AA516" t="s">
+        <v>124</v>
+      </c>
+      <c r="AB516" t="s">
+        <v>43</v>
+      </c>
+      <c r="AC516" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="517" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A517" s="7">
+        <v>200</v>
+      </c>
+      <c r="B517" t="s">
+        <v>129</v>
+      </c>
+      <c r="C517" t="s">
+        <v>130</v>
+      </c>
+      <c r="D517" t="s">
+        <v>66</v>
+      </c>
+      <c r="E517" t="s">
+        <v>32</v>
+      </c>
+      <c r="F517" s="3">
+        <v>46023</v>
+      </c>
+      <c r="G517">
+        <v>2026</v>
+      </c>
+      <c r="H517" t="s">
+        <v>518</v>
+      </c>
+      <c r="I517" t="s">
+        <v>518</v>
+      </c>
+      <c r="J517">
+        <v>2</v>
+      </c>
+      <c r="K517">
+        <v>80</v>
+      </c>
+      <c r="L517">
+        <v>87.4</v>
+      </c>
+      <c r="M517">
+        <f>+L517/K517</f>
+        <v>1.0925</v>
+      </c>
+      <c r="N517">
+        <v>1.0925</v>
+      </c>
+      <c r="O517" t="s">
+        <v>58</v>
+      </c>
+      <c r="P517" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q517" t="s">
+        <v>512</v>
+      </c>
+      <c r="R517">
+        <v>0</v>
+      </c>
+      <c r="S517">
+        <v>1</v>
+      </c>
+      <c r="T517" t="s">
+        <v>518</v>
+      </c>
+      <c r="U517" t="s">
+        <v>37</v>
+      </c>
+      <c r="V517" t="s">
+        <v>130</v>
+      </c>
+      <c r="W517" t="s">
+        <v>60</v>
+      </c>
+      <c r="X517" t="s">
+        <v>100</v>
+      </c>
+      <c r="Y517" t="s">
+        <v>133</v>
+      </c>
+      <c r="Z517" t="s">
+        <v>134</v>
+      </c>
+      <c r="AA517" t="s">
+        <v>135</v>
+      </c>
+      <c r="AB517" t="s">
+        <v>43</v>
+      </c>
+      <c r="AC517" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="518" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A518">
+        <v>202</v>
+      </c>
+      <c r="B518" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="C518" t="s">
+        <v>130</v>
+      </c>
+      <c r="D518" t="s">
+        <v>66</v>
+      </c>
+      <c r="E518" t="s">
+        <v>32</v>
+      </c>
+      <c r="F518" s="3">
+        <v>46023</v>
+      </c>
+      <c r="G518">
+        <v>2026</v>
+      </c>
+      <c r="H518" t="s">
+        <v>518</v>
+      </c>
+      <c r="I518" t="s">
+        <v>518</v>
+      </c>
+      <c r="K518">
+        <v>68.7</v>
+      </c>
+      <c r="L518">
+        <v>81</v>
+      </c>
+      <c r="M518">
+        <f>+L518/K518</f>
+        <v>1.1790393013100435</v>
+      </c>
+      <c r="N518">
+        <f>+L518/K518</f>
+        <v>1.1790393013100435</v>
+      </c>
+      <c r="O518" t="s">
+        <v>245</v>
+      </c>
+      <c r="P518" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q518" t="s">
+        <v>513</v>
+      </c>
+      <c r="R518">
+        <v>1</v>
+      </c>
+      <c r="S518">
+        <v>1</v>
+      </c>
+      <c r="T518" t="s">
+        <v>518</v>
+      </c>
+      <c r="U518" t="s">
+        <v>37</v>
+      </c>
+      <c r="V518" t="s">
+        <v>130</v>
+      </c>
+      <c r="W518" t="s">
+        <v>60</v>
+      </c>
+      <c r="X518" t="s">
+        <v>100</v>
+      </c>
+      <c r="Y518" t="s">
+        <v>139</v>
+      </c>
+      <c r="Z518" t="s">
+        <v>63</v>
+      </c>
+      <c r="AA518" t="s">
+        <v>115</v>
+      </c>
+      <c r="AB518" t="s">
+        <v>43</v>
+      </c>
+      <c r="AC518" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="519" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A519">
+        <v>203</v>
+      </c>
+      <c r="B519" t="s">
+        <v>141</v>
+      </c>
+      <c r="C519" t="s">
+        <v>142</v>
+      </c>
+      <c r="D519" t="s">
+        <v>31</v>
+      </c>
+      <c r="E519" t="s">
+        <v>32</v>
+      </c>
+      <c r="F519" s="3">
+        <v>46023</v>
+      </c>
+      <c r="G519">
+        <v>2026</v>
+      </c>
+      <c r="H519" t="s">
+        <v>518</v>
+      </c>
+      <c r="I519" t="s">
+        <v>518</v>
+      </c>
+      <c r="K519">
+        <f>+K203+K206+K209+K479</f>
+        <v>1088227.5892360001</v>
+      </c>
+      <c r="L519">
+        <f>+L203+L206+L209+L479</f>
+        <v>1146226.222453973</v>
+      </c>
+      <c r="M519">
+        <f t="shared" ref="M519" si="94">+L519/K519</f>
+        <v>1.053296418682687</v>
+      </c>
+      <c r="N519">
+        <f t="shared" ref="N519" si="95">+L519/K519</f>
+        <v>1.053296418682687</v>
+      </c>
+      <c r="O519" t="s">
+        <v>143</v>
+      </c>
+      <c r="P519" t="s">
+        <v>143</v>
+      </c>
+      <c r="Q519" t="str">
+        <f>A519&amp;"-"&amp;TEXT(F519,"yyyy-mm-dd")</f>
+        <v>203-2026-01-01</v>
+      </c>
+      <c r="R519">
+        <v>0</v>
+      </c>
+      <c r="S519">
+        <v>0</v>
+      </c>
+      <c r="T519" t="s">
+        <v>518</v>
+      </c>
+      <c r="U519" t="s">
+        <v>37</v>
+      </c>
+      <c r="V519" t="s">
+        <v>142</v>
+      </c>
+      <c r="W519" t="s">
+        <v>145</v>
+      </c>
+      <c r="X519" t="s">
+        <v>146</v>
+      </c>
+      <c r="Y519" t="s">
+        <v>147</v>
+      </c>
+      <c r="Z519" t="s">
+        <v>63</v>
+      </c>
+      <c r="AA519" t="s">
+        <v>148</v>
+      </c>
+      <c r="AB519" t="s">
+        <v>78</v>
+      </c>
+      <c r="AC519" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="520" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A520">
+        <v>204</v>
+      </c>
+      <c r="B520" t="s">
+        <v>154</v>
+      </c>
+      <c r="C520" t="s">
+        <v>142</v>
+      </c>
+      <c r="D520" t="s">
+        <v>31</v>
+      </c>
+      <c r="E520" t="s">
+        <v>32</v>
+      </c>
+      <c r="F520" s="3">
+        <v>46023</v>
+      </c>
+      <c r="G520">
+        <v>2026</v>
+      </c>
+      <c r="H520" t="s">
+        <v>518</v>
+      </c>
+      <c r="I520" t="s">
+        <v>518</v>
+      </c>
+      <c r="L520">
+        <f>128448131182/1000000</f>
+        <v>128448.131182</v>
+      </c>
+      <c r="O520" t="s">
+        <v>143</v>
+      </c>
+      <c r="P520" t="s">
+        <v>143</v>
+      </c>
+      <c r="Q520" t="s">
+        <v>496</v>
+      </c>
+      <c r="R520">
+        <v>0</v>
+      </c>
+      <c r="S520">
+        <v>0</v>
+      </c>
+      <c r="T520" t="s">
+        <v>518</v>
+      </c>
+      <c r="U520" t="s">
+        <v>37</v>
+      </c>
+      <c r="V520" t="s">
+        <v>142</v>
+      </c>
+      <c r="W520" t="s">
+        <v>145</v>
+      </c>
+      <c r="X520" t="s">
+        <v>146</v>
+      </c>
+      <c r="Y520" t="s">
+        <v>147</v>
+      </c>
+      <c r="Z520" t="s">
+        <v>63</v>
+      </c>
+      <c r="AA520" t="s">
+        <v>148</v>
+      </c>
+      <c r="AB520" t="s">
+        <v>43</v>
+      </c>
+      <c r="AC520" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="521" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A521">
+        <v>205</v>
+      </c>
+      <c r="B521" t="s">
+        <v>161</v>
+      </c>
+      <c r="C521" t="s">
+        <v>142</v>
+      </c>
+      <c r="D521" t="s">
+        <v>31</v>
+      </c>
+      <c r="E521" t="s">
+        <v>32</v>
+      </c>
+      <c r="F521" s="3">
+        <v>46023</v>
+      </c>
+      <c r="G521">
+        <v>2026</v>
+      </c>
+      <c r="H521" t="s">
+        <v>518</v>
+      </c>
+      <c r="I521" t="s">
+        <v>518</v>
+      </c>
+      <c r="K521">
+        <v>4684</v>
+      </c>
+      <c r="L521">
+        <v>4684</v>
+      </c>
+      <c r="M521">
+        <v>1.3</v>
+      </c>
+      <c r="N521">
+        <v>1.8631019332578229</v>
+      </c>
+      <c r="O521" t="s">
+        <v>143</v>
+      </c>
+      <c r="P521" t="s">
+        <v>143</v>
+      </c>
+      <c r="Q521" t="s">
+        <v>422</v>
+      </c>
+      <c r="R521">
+        <v>0</v>
+      </c>
+      <c r="S521">
+        <v>0</v>
+      </c>
+      <c r="T521" t="s">
+        <v>518</v>
+      </c>
+      <c r="U521" t="s">
+        <v>37</v>
+      </c>
+      <c r="V521" t="s">
+        <v>142</v>
+      </c>
+      <c r="W521" t="s">
+        <v>145</v>
+      </c>
+      <c r="X521" t="s">
+        <v>146</v>
+      </c>
+      <c r="Y521" t="s">
+        <v>147</v>
+      </c>
+      <c r="Z521" t="s">
+        <v>63</v>
+      </c>
+      <c r="AA521" t="s">
+        <v>148</v>
+      </c>
+      <c r="AB521" t="s">
+        <v>78</v>
+      </c>
+      <c r="AC521" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="522" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A522">
+        <v>244</v>
+      </c>
+      <c r="B522" t="s">
+        <v>182</v>
+      </c>
+      <c r="C522" t="s">
+        <v>177</v>
+      </c>
+      <c r="D522" t="s">
+        <v>66</v>
+      </c>
+      <c r="E522" t="s">
+        <v>171</v>
+      </c>
+      <c r="F522" s="3">
+        <v>46023</v>
+      </c>
+      <c r="G522">
+        <v>2026</v>
+      </c>
+      <c r="H522" t="s">
+        <v>518</v>
+      </c>
+      <c r="I522" t="s">
+        <v>518</v>
+      </c>
+      <c r="K522">
+        <v>25</v>
+      </c>
+      <c r="L522">
+        <v>13</v>
+      </c>
+      <c r="M522">
+        <f>IF(K522/L522&gt;1.3,1.3,K522/L522)</f>
+        <v>1.3</v>
+      </c>
+      <c r="N522">
+        <f>+K522/L522</f>
+        <v>1.9230769230769231</v>
+      </c>
+      <c r="O522" t="s">
+        <v>35</v>
+      </c>
+      <c r="P522" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q522" t="s">
+        <v>501</v>
+      </c>
+      <c r="R522">
+        <v>0</v>
+      </c>
+      <c r="S522">
+        <v>0</v>
+      </c>
+      <c r="T522" t="s">
+        <v>518</v>
+      </c>
+      <c r="U522" t="s">
+        <v>37</v>
+      </c>
+      <c r="V522" t="s">
+        <v>177</v>
+      </c>
+      <c r="W522" t="s">
+        <v>145</v>
+      </c>
+      <c r="X522" t="s">
+        <v>179</v>
+      </c>
+      <c r="Y522" t="s">
+        <v>180</v>
+      </c>
+      <c r="Z522" t="s">
+        <v>63</v>
+      </c>
+      <c r="AA522" t="s">
+        <v>64</v>
+      </c>
+      <c r="AB522" t="s">
+        <v>43</v>
+      </c>
+      <c r="AC522" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="523" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A523">
+        <v>245</v>
+      </c>
+      <c r="B523" t="s">
+        <v>185</v>
+      </c>
+      <c r="C523" t="s">
+        <v>186</v>
+      </c>
+      <c r="D523" t="s">
+        <v>31</v>
+      </c>
+      <c r="E523" t="s">
+        <v>32</v>
+      </c>
+      <c r="F523" s="3">
+        <v>46023</v>
+      </c>
+      <c r="G523">
+        <v>2026</v>
+      </c>
+      <c r="H523" t="s">
+        <v>518</v>
+      </c>
+      <c r="I523" t="s">
+        <v>518</v>
+      </c>
+      <c r="K523">
+        <v>86.1</v>
+      </c>
+      <c r="L523">
+        <v>86.2</v>
+      </c>
+      <c r="M523">
+        <f t="shared" ref="M523:M524" si="96">+L523/K523</f>
+        <v>1.0011614401858304</v>
+      </c>
+      <c r="N523">
+        <f t="shared" ref="N523:N524" si="97">+L523/K523</f>
+        <v>1.0011614401858304</v>
+      </c>
+      <c r="O523" t="s">
+        <v>58</v>
+      </c>
+      <c r="P523" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q523" t="s">
+        <v>421</v>
+      </c>
+      <c r="R523">
+        <v>1</v>
+      </c>
+      <c r="S523">
+        <v>1</v>
+      </c>
+      <c r="T523" t="s">
+        <v>518</v>
+      </c>
+      <c r="U523" t="s">
+        <v>37</v>
+      </c>
+      <c r="V523" t="s">
+        <v>186</v>
+      </c>
+      <c r="W523" t="s">
+        <v>112</v>
+      </c>
+      <c r="X523" t="s">
+        <v>113</v>
+      </c>
+      <c r="Y523" t="s">
+        <v>123</v>
+      </c>
+      <c r="Z523" t="s">
+        <v>41</v>
+      </c>
+      <c r="AA523" t="s">
+        <v>42</v>
+      </c>
+      <c r="AB523" t="s">
+        <v>65</v>
+      </c>
+      <c r="AC523" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="524" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A524">
+        <v>274</v>
+      </c>
+      <c r="B524" t="s">
+        <v>480</v>
+      </c>
+      <c r="C524" t="s">
+        <v>194</v>
+      </c>
+      <c r="D524" t="s">
+        <v>31</v>
+      </c>
+      <c r="E524" t="s">
+        <v>32</v>
+      </c>
+      <c r="F524" s="3">
+        <v>46023</v>
+      </c>
+      <c r="G524">
+        <v>2026</v>
+      </c>
+      <c r="H524" t="s">
+        <v>518</v>
+      </c>
+      <c r="I524" t="s">
+        <v>518</v>
+      </c>
+      <c r="K524">
+        <v>44737</v>
+      </c>
+      <c r="L524" s="4">
+        <v>45646</v>
+      </c>
+      <c r="M524">
+        <f t="shared" si="96"/>
+        <v>1.02031875181617</v>
+      </c>
+      <c r="N524">
+        <f t="shared" si="97"/>
+        <v>1.02031875181617</v>
+      </c>
+      <c r="O524" t="s">
+        <v>35</v>
+      </c>
+      <c r="P524" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q524" t="str">
+        <f>A524&amp;"-"&amp;TEXT(F524,"yyyy-mm-dd")</f>
+        <v>274-2026-01-01</v>
+      </c>
+      <c r="R524">
+        <v>0</v>
+      </c>
+      <c r="S524">
+        <v>0</v>
+      </c>
+      <c r="T524" t="s">
+        <v>518</v>
+      </c>
+      <c r="U524" t="s">
+        <v>37</v>
+      </c>
+      <c r="V524" t="s">
+        <v>194</v>
+      </c>
+      <c r="W524" t="s">
+        <v>38</v>
+      </c>
+      <c r="X524" t="s">
+        <v>39</v>
+      </c>
+      <c r="Y524" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z524" t="s">
+        <v>41</v>
+      </c>
+      <c r="AA524" t="s">
+        <v>42</v>
+      </c>
+      <c r="AB524" t="s">
+        <v>78</v>
+      </c>
+      <c r="AC524" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="525" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A525">
+        <v>276</v>
+      </c>
+      <c r="B525" t="s">
+        <v>201</v>
+      </c>
+      <c r="C525" t="s">
+        <v>202</v>
+      </c>
+      <c r="D525" t="s">
+        <v>31</v>
+      </c>
+      <c r="E525" t="s">
+        <v>171</v>
+      </c>
+      <c r="F525" s="3">
+        <v>46023</v>
+      </c>
+      <c r="G525">
+        <v>2026</v>
+      </c>
+      <c r="H525" t="s">
+        <v>518</v>
+      </c>
+      <c r="I525" t="s">
+        <v>518</v>
+      </c>
+      <c r="K525">
+        <v>81</v>
+      </c>
+      <c r="L525">
+        <v>82.81</v>
+      </c>
+      <c r="M525">
+        <f t="shared" ref="M525:M526" si="98">+K525/L525</f>
+        <v>0.97814273638449456</v>
+      </c>
+      <c r="N525">
+        <f t="shared" ref="N525:N526" si="99">+K525/L525</f>
+        <v>0.97814273638449456</v>
+      </c>
+      <c r="O525" t="s">
+        <v>35</v>
+      </c>
+      <c r="P525" t="s">
+        <v>245</v>
+      </c>
+      <c r="Q525" t="s">
+        <v>514</v>
+      </c>
+      <c r="R525">
+        <v>0</v>
+      </c>
+      <c r="S525">
+        <v>1</v>
+      </c>
+      <c r="T525" t="s">
+        <v>518</v>
+      </c>
+      <c r="U525" t="s">
+        <v>37</v>
+      </c>
+      <c r="V525" t="s">
+        <v>202</v>
+      </c>
+      <c r="W525" t="s">
+        <v>73</v>
+      </c>
+      <c r="X525" t="s">
+        <v>74</v>
+      </c>
+      <c r="Y525" t="s">
+        <v>75</v>
+      </c>
+      <c r="Z525" t="s">
+        <v>86</v>
+      </c>
+      <c r="AA525" t="s">
+        <v>204</v>
+      </c>
+      <c r="AB525" t="s">
+        <v>65</v>
+      </c>
+      <c r="AC525" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="526" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A526">
+        <v>277</v>
+      </c>
+      <c r="B526" t="s">
+        <v>210</v>
+      </c>
+      <c r="C526" t="s">
+        <v>202</v>
+      </c>
+      <c r="D526" t="s">
+        <v>31</v>
+      </c>
+      <c r="E526" t="s">
+        <v>171</v>
+      </c>
+      <c r="F526" s="3">
+        <v>46023</v>
+      </c>
+      <c r="G526">
+        <v>2026</v>
+      </c>
+      <c r="H526" t="s">
+        <v>518</v>
+      </c>
+      <c r="I526" t="s">
+        <v>518</v>
+      </c>
+      <c r="K526">
+        <v>71</v>
+      </c>
+      <c r="L526">
+        <v>68.400000000000006</v>
+      </c>
+      <c r="M526">
+        <f t="shared" si="98"/>
+        <v>1.0380116959064327</v>
+      </c>
+      <c r="N526">
+        <f t="shared" si="99"/>
+        <v>1.0380116959064327</v>
+      </c>
+      <c r="O526" t="s">
+        <v>35</v>
+      </c>
+      <c r="P526" t="s">
+        <v>245</v>
+      </c>
+      <c r="Q526" t="s">
+        <v>515</v>
+      </c>
+      <c r="R526">
+        <v>1</v>
+      </c>
+      <c r="S526">
+        <v>1</v>
+      </c>
+      <c r="T526" t="s">
+        <v>518</v>
+      </c>
+      <c r="U526" t="s">
+        <v>37</v>
+      </c>
+      <c r="V526" t="s">
+        <v>202</v>
+      </c>
+      <c r="W526" t="s">
+        <v>73</v>
+      </c>
+      <c r="X526" t="s">
+        <v>74</v>
+      </c>
+      <c r="Z526" t="s">
+        <v>86</v>
+      </c>
+      <c r="AA526" t="s">
+        <v>204</v>
+      </c>
+      <c r="AB526" t="s">
+        <v>65</v>
+      </c>
+      <c r="AC526" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="527" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A527">
+        <v>332</v>
+      </c>
+      <c r="B527" t="s">
+        <v>239</v>
+      </c>
+      <c r="C527" t="s">
+        <v>130</v>
+      </c>
+      <c r="D527" t="s">
+        <v>31</v>
+      </c>
+      <c r="E527" t="s">
+        <v>171</v>
+      </c>
+      <c r="F527" s="3">
+        <v>45838</v>
+      </c>
+      <c r="G527">
+        <v>2025</v>
+      </c>
+      <c r="H527" t="s">
+        <v>33</v>
+      </c>
+      <c r="I527" t="s">
+        <v>404</v>
+      </c>
+      <c r="K527">
+        <v>1.4</v>
+      </c>
+      <c r="L527">
+        <v>0.85</v>
+      </c>
+      <c r="M527">
+        <v>1.3</v>
+      </c>
+      <c r="N527">
+        <v>1.6470588235294119</v>
+      </c>
+      <c r="O527" t="s">
+        <v>245</v>
+      </c>
+      <c r="P527" t="s">
+        <v>245</v>
+      </c>
+      <c r="Q527" t="s">
+        <v>431</v>
+      </c>
+      <c r="R527">
+        <v>2</v>
+      </c>
+      <c r="S527">
+        <v>2</v>
+      </c>
+      <c r="T527" t="s">
+        <v>443</v>
+      </c>
+      <c r="U527" t="s">
+        <v>37</v>
+      </c>
+      <c r="V527" t="s">
+        <v>130</v>
+      </c>
+      <c r="W527" t="s">
+        <v>60</v>
+      </c>
+      <c r="X527" t="s">
+        <v>100</v>
+      </c>
+      <c r="Y527" t="s">
+        <v>241</v>
+      </c>
+      <c r="Z527" t="s">
+        <v>134</v>
+      </c>
+      <c r="AA527" t="s">
+        <v>135</v>
+      </c>
+      <c r="AB527" t="s">
+        <v>65</v>
+      </c>
+      <c r="AC527" t="s">
+        <v>66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Feat: Ajustar cascada y filtros para datos de Avance 2026
- Incluir año 2026 en filtros (datos de Avance están en 2026)
- Dashboard: Cascada simplificada a 2 niveles (Línea → Objetivo)
- Análisis por Línea: Cascada con 3 niveles (Línea → Objetivo → Meta PDI)
- Agregar gráfico sunburst en Análisis por Línea
- Mostrar métricas en 0 cuando no hay datos disponibles
- Agregar parámetro max_niveles a obtener_cumplimiento_cascada()

Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/Data/Dataset_Unificado.xlsx
+++ b/Data/Dataset_Unificado.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5f15395a9ed9a48f/Proyectos_DS/PDI_2022_2025/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2175" documentId="11_C54DB9D477E07092D1C9E253F65DD242EE9209D1" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{47272230-57A3-4A1B-8397-976C1A73F68E}"/>
+  <xr:revisionPtr revIDLastSave="2244" documentId="11_C54DB9D477E07092D1C9E253F65DD242EE9209D1" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{776C814E-F7F9-406C-8AA9-212BF40FB006}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Base_Indicadores!$A$1:$M$58</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Unificado!$A$1:$AC$526</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Unificado!$A$1:$AC$539</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14696" uniqueCount="520">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14915" uniqueCount="520">
   <si>
     <t>Id</t>
   </si>
@@ -2005,11 +2005,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AC527"/>
+  <dimension ref="A1:AC539"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -15418,7 +15416,7 @@
         <v>1.3</v>
       </c>
       <c r="N156">
-        <f t="shared" ref="N156:N163" si="25">+L156/K156</f>
+        <f t="shared" ref="N156:N162" si="25">+L156/K156</f>
         <v>1.4279999999999999</v>
       </c>
       <c r="O156" t="s">
@@ -45634,9 +45632,6 @@
       <c r="I501" t="s">
         <v>465</v>
       </c>
-      <c r="J501">
-        <v>2</v>
-      </c>
       <c r="K501">
         <v>83197</v>
       </c>
@@ -46703,7 +46698,7 @@
         <v>94</v>
       </c>
       <c r="M513">
-        <f t="shared" ref="M513:M514" si="91">+L513/K513</f>
+        <f t="shared" ref="M513" si="91">+L513/K513</f>
         <v>1.175</v>
       </c>
       <c r="N513">
@@ -47907,16 +47902,16 @@
         <v>171</v>
       </c>
       <c r="F527" s="3">
-        <v>45838</v>
+        <v>46023</v>
       </c>
       <c r="G527">
-        <v>2025</v>
+        <v>2026</v>
       </c>
       <c r="H527" t="s">
-        <v>33</v>
+        <v>518</v>
       </c>
       <c r="I527" t="s">
-        <v>404</v>
+        <v>518</v>
       </c>
       <c r="K527">
         <v>1.4</v>
@@ -47946,7 +47941,7 @@
         <v>2</v>
       </c>
       <c r="T527" t="s">
-        <v>443</v>
+        <v>518</v>
       </c>
       <c r="U527" t="s">
         <v>37</v>
@@ -47973,6 +47968,1055 @@
         <v>65</v>
       </c>
       <c r="AC527" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="528" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A528">
+        <v>364</v>
+      </c>
+      <c r="B528" t="s">
+        <v>271</v>
+      </c>
+      <c r="C528" t="s">
+        <v>267</v>
+      </c>
+      <c r="D528" t="s">
+        <v>31</v>
+      </c>
+      <c r="E528" t="s">
+        <v>171</v>
+      </c>
+      <c r="F528" s="3">
+        <v>46023</v>
+      </c>
+      <c r="G528">
+        <v>2026</v>
+      </c>
+      <c r="H528" t="s">
+        <v>518</v>
+      </c>
+      <c r="I528" t="s">
+        <v>518</v>
+      </c>
+      <c r="K528">
+        <f>+K369+K501</f>
+        <v>162432</v>
+      </c>
+      <c r="L528">
+        <f>+L369+L501</f>
+        <v>158937</v>
+      </c>
+      <c r="M528">
+        <f t="shared" ref="M528" si="100">+L528/K528</f>
+        <v>0.97848330378250592</v>
+      </c>
+      <c r="N528">
+        <f t="shared" ref="N528" si="101">+L528/K528</f>
+        <v>0.97848330378250592</v>
+      </c>
+      <c r="O528" t="s">
+        <v>35</v>
+      </c>
+      <c r="P528" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q528" t="s">
+        <v>516</v>
+      </c>
+      <c r="R528">
+        <v>0</v>
+      </c>
+      <c r="S528">
+        <v>0</v>
+      </c>
+      <c r="T528" t="s">
+        <v>518</v>
+      </c>
+      <c r="U528" t="s">
+        <v>37</v>
+      </c>
+      <c r="V528" t="s">
+        <v>267</v>
+      </c>
+      <c r="W528" t="s">
+        <v>145</v>
+      </c>
+      <c r="X528" t="s">
+        <v>179</v>
+      </c>
+      <c r="Y528" t="s">
+        <v>273</v>
+      </c>
+      <c r="Z528" t="s">
+        <v>274</v>
+      </c>
+      <c r="AA528" t="s">
+        <v>275</v>
+      </c>
+      <c r="AB528" t="s">
+        <v>78</v>
+      </c>
+      <c r="AC528" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="529" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A529">
+        <v>367</v>
+      </c>
+      <c r="B529" t="s">
+        <v>500</v>
+      </c>
+      <c r="C529" t="s">
+        <v>267</v>
+      </c>
+      <c r="D529" t="s">
+        <v>66</v>
+      </c>
+      <c r="E529" t="s">
+        <v>32</v>
+      </c>
+      <c r="F529" s="3">
+        <v>46023</v>
+      </c>
+      <c r="G529">
+        <v>2026</v>
+      </c>
+      <c r="H529" t="s">
+        <v>518</v>
+      </c>
+      <c r="I529" t="s">
+        <v>518</v>
+      </c>
+      <c r="K529">
+        <v>5</v>
+      </c>
+      <c r="L529">
+        <v>5.43</v>
+      </c>
+      <c r="M529">
+        <f>+L529/K529</f>
+        <v>1.0859999999999999</v>
+      </c>
+      <c r="N529">
+        <f>+L529/K529</f>
+        <v>1.0859999999999999</v>
+      </c>
+      <c r="O529" t="s">
+        <v>58</v>
+      </c>
+      <c r="P529" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q529" t="s">
+        <v>499</v>
+      </c>
+      <c r="R529">
+        <v>1</v>
+      </c>
+      <c r="S529">
+        <v>2</v>
+      </c>
+      <c r="T529" t="s">
+        <v>518</v>
+      </c>
+      <c r="U529" t="s">
+        <v>37</v>
+      </c>
+      <c r="V529" t="s">
+        <v>267</v>
+      </c>
+      <c r="W529" t="s">
+        <v>145</v>
+      </c>
+      <c r="X529" t="s">
+        <v>179</v>
+      </c>
+      <c r="Y529" t="s">
+        <v>281</v>
+      </c>
+      <c r="Z529" t="s">
+        <v>41</v>
+      </c>
+      <c r="AA529" t="s">
+        <v>42</v>
+      </c>
+      <c r="AB529" t="s">
+        <v>43</v>
+      </c>
+      <c r="AC529" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="530" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A530">
+        <v>369</v>
+      </c>
+      <c r="B530" t="s">
+        <v>283</v>
+      </c>
+      <c r="C530" t="s">
+        <v>267</v>
+      </c>
+      <c r="D530" t="s">
+        <v>31</v>
+      </c>
+      <c r="E530" t="s">
+        <v>32</v>
+      </c>
+      <c r="F530" s="3">
+        <v>46023</v>
+      </c>
+      <c r="G530">
+        <v>2026</v>
+      </c>
+      <c r="H530" t="s">
+        <v>518</v>
+      </c>
+      <c r="I530" t="s">
+        <v>518</v>
+      </c>
+      <c r="K530">
+        <f>+K502+K383</f>
+        <v>378</v>
+      </c>
+      <c r="L530">
+        <f>+L502+L383</f>
+        <v>328</v>
+      </c>
+      <c r="M530">
+        <f t="shared" ref="M530:M531" si="102">+L530/K530</f>
+        <v>0.86772486772486768</v>
+      </c>
+      <c r="N530">
+        <f>+L530/K530</f>
+        <v>0.86772486772486768</v>
+      </c>
+      <c r="O530" t="s">
+        <v>35</v>
+      </c>
+      <c r="P530" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q530" t="s">
+        <v>517</v>
+      </c>
+      <c r="R530">
+        <v>0</v>
+      </c>
+      <c r="S530">
+        <v>0</v>
+      </c>
+      <c r="T530" t="s">
+        <v>518</v>
+      </c>
+      <c r="U530" t="s">
+        <v>37</v>
+      </c>
+      <c r="V530" t="s">
+        <v>267</v>
+      </c>
+      <c r="W530" t="s">
+        <v>145</v>
+      </c>
+      <c r="X530" t="s">
+        <v>179</v>
+      </c>
+      <c r="Y530" t="s">
+        <v>273</v>
+      </c>
+      <c r="Z530" t="s">
+        <v>41</v>
+      </c>
+      <c r="AA530" t="s">
+        <v>42</v>
+      </c>
+      <c r="AB530" t="s">
+        <v>78</v>
+      </c>
+      <c r="AC530" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="531" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A531">
+        <v>376</v>
+      </c>
+      <c r="B531" t="s">
+        <v>473</v>
+      </c>
+      <c r="C531" t="s">
+        <v>142</v>
+      </c>
+      <c r="D531" t="s">
+        <v>31</v>
+      </c>
+      <c r="E531" t="s">
+        <v>32</v>
+      </c>
+      <c r="F531" s="3">
+        <v>46023</v>
+      </c>
+      <c r="G531">
+        <v>2026</v>
+      </c>
+      <c r="H531" t="s">
+        <v>518</v>
+      </c>
+      <c r="I531" t="s">
+        <v>518</v>
+      </c>
+      <c r="K531">
+        <f>+K393+K391+K389+K387</f>
+        <v>101274.06472913575</v>
+      </c>
+      <c r="L531">
+        <f>+L393+L391+L389+L387</f>
+        <v>112137.89274782965</v>
+      </c>
+      <c r="M531">
+        <f t="shared" si="102"/>
+        <v>1.1072715709372378</v>
+      </c>
+      <c r="N531">
+        <f t="shared" ref="N531" si="103">+L531/K531</f>
+        <v>1.1072715709372378</v>
+      </c>
+      <c r="O531" t="s">
+        <v>143</v>
+      </c>
+      <c r="P531" t="s">
+        <v>143</v>
+      </c>
+      <c r="Q531" t="s">
+        <v>498</v>
+      </c>
+      <c r="R531">
+        <v>0</v>
+      </c>
+      <c r="S531">
+        <v>0</v>
+      </c>
+      <c r="T531" t="s">
+        <v>518</v>
+      </c>
+      <c r="U531" t="s">
+        <v>37</v>
+      </c>
+      <c r="V531" t="s">
+        <v>142</v>
+      </c>
+      <c r="W531" t="s">
+        <v>145</v>
+      </c>
+      <c r="X531" t="s">
+        <v>146</v>
+      </c>
+      <c r="Y531" t="s">
+        <v>147</v>
+      </c>
+      <c r="Z531" t="s">
+        <v>63</v>
+      </c>
+      <c r="AA531" t="s">
+        <v>148</v>
+      </c>
+      <c r="AB531" t="s">
+        <v>78</v>
+      </c>
+      <c r="AC531" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="532" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A532">
+        <v>379</v>
+      </c>
+      <c r="B532" t="s">
+        <v>301</v>
+      </c>
+      <c r="C532" t="s">
+        <v>302</v>
+      </c>
+      <c r="D532" t="s">
+        <v>31</v>
+      </c>
+      <c r="E532" t="s">
+        <v>32</v>
+      </c>
+      <c r="F532" s="3">
+        <v>46023</v>
+      </c>
+      <c r="G532">
+        <v>2026</v>
+      </c>
+      <c r="H532" t="s">
+        <v>518</v>
+      </c>
+      <c r="I532" t="s">
+        <v>518</v>
+      </c>
+      <c r="K532">
+        <f>+K413+K416+K419+K503</f>
+        <v>90899</v>
+      </c>
+      <c r="L532">
+        <f>+L413+L416+L419+L503</f>
+        <v>92559</v>
+      </c>
+      <c r="M532">
+        <f>+L532/K532</f>
+        <v>1.0182620270850065</v>
+      </c>
+      <c r="N532">
+        <f>+L532/K532</f>
+        <v>1.0182620270850065</v>
+      </c>
+      <c r="O532" t="s">
+        <v>35</v>
+      </c>
+      <c r="P532" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q532" t="str">
+        <f>A532&amp;"-"&amp;TEXT(F532,"yyyy-mm-dd")</f>
+        <v>379-2026-01-01</v>
+      </c>
+      <c r="R532">
+        <v>0</v>
+      </c>
+      <c r="S532">
+        <v>0</v>
+      </c>
+      <c r="T532" t="s">
+        <v>518</v>
+      </c>
+      <c r="U532" t="s">
+        <v>37</v>
+      </c>
+      <c r="V532" t="s">
+        <v>302</v>
+      </c>
+      <c r="W532" t="s">
+        <v>38</v>
+      </c>
+      <c r="X532" t="s">
+        <v>39</v>
+      </c>
+      <c r="Y532" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z532" t="s">
+        <v>41</v>
+      </c>
+      <c r="AA532" t="s">
+        <v>42</v>
+      </c>
+      <c r="AB532" t="s">
+        <v>78</v>
+      </c>
+      <c r="AC532" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="533" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A533">
+        <v>385</v>
+      </c>
+      <c r="B533" t="s">
+        <v>309</v>
+      </c>
+      <c r="C533" t="s">
+        <v>310</v>
+      </c>
+      <c r="D533" t="s">
+        <v>31</v>
+      </c>
+      <c r="E533" t="s">
+        <v>32</v>
+      </c>
+      <c r="F533" s="3">
+        <v>46023</v>
+      </c>
+      <c r="G533">
+        <v>2026</v>
+      </c>
+      <c r="H533" t="s">
+        <v>518</v>
+      </c>
+      <c r="I533" t="s">
+        <v>518</v>
+      </c>
+      <c r="K533">
+        <f>+K484+K427+K425+K423</f>
+        <v>60024.456511000004</v>
+      </c>
+      <c r="L533">
+        <f>+L484+L427+L425+L423</f>
+        <v>58331.780656999996</v>
+      </c>
+      <c r="M533">
+        <f>L533/K533</f>
+        <v>0.97180023023299156</v>
+      </c>
+      <c r="N533">
+        <f>L533/K533</f>
+        <v>0.97180023023299156</v>
+      </c>
+      <c r="O533" t="s">
+        <v>143</v>
+      </c>
+      <c r="P533" t="s">
+        <v>143</v>
+      </c>
+      <c r="Q533" t="s">
+        <v>486</v>
+      </c>
+      <c r="R533">
+        <v>0</v>
+      </c>
+      <c r="S533">
+        <v>0</v>
+      </c>
+      <c r="T533" t="s">
+        <v>518</v>
+      </c>
+      <c r="U533" t="s">
+        <v>37</v>
+      </c>
+      <c r="V533" t="s">
+        <v>310</v>
+      </c>
+      <c r="W533" t="s">
+        <v>312</v>
+      </c>
+      <c r="X533" t="s">
+        <v>313</v>
+      </c>
+      <c r="Y533" t="s">
+        <v>314</v>
+      </c>
+      <c r="AB533" t="s">
+        <v>43</v>
+      </c>
+      <c r="AC533" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="534" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A534">
+        <v>386.1</v>
+      </c>
+      <c r="B534" t="s">
+        <v>377</v>
+      </c>
+      <c r="C534" t="s">
+        <v>310</v>
+      </c>
+      <c r="D534" t="s">
+        <v>31</v>
+      </c>
+      <c r="E534" t="s">
+        <v>32</v>
+      </c>
+      <c r="F534" s="3">
+        <v>46023</v>
+      </c>
+      <c r="G534">
+        <v>2026</v>
+      </c>
+      <c r="H534" t="s">
+        <v>518</v>
+      </c>
+      <c r="I534" t="s">
+        <v>518</v>
+      </c>
+      <c r="K534">
+        <f>+K483+K434+K432+K430</f>
+        <v>9719.0247151999993</v>
+      </c>
+      <c r="L534">
+        <f>+L483+L434+L432+L430</f>
+        <v>12435.92103</v>
+      </c>
+      <c r="M534">
+        <f>IF(+L534/K534&gt;1.3,1.3,L534/K534)</f>
+        <v>1.2795441306524233</v>
+      </c>
+      <c r="N534">
+        <f>+L534/K534</f>
+        <v>1.2795441306524233</v>
+      </c>
+      <c r="O534" t="s">
+        <v>143</v>
+      </c>
+      <c r="P534" t="s">
+        <v>143</v>
+      </c>
+      <c r="Q534" t="s">
+        <v>490</v>
+      </c>
+      <c r="R534">
+        <v>0</v>
+      </c>
+      <c r="S534">
+        <v>0</v>
+      </c>
+      <c r="T534" t="s">
+        <v>518</v>
+      </c>
+      <c r="U534" t="s">
+        <v>37</v>
+      </c>
+      <c r="V534" t="s">
+        <v>310</v>
+      </c>
+      <c r="W534" t="s">
+        <v>312</v>
+      </c>
+      <c r="X534" t="s">
+        <v>313</v>
+      </c>
+      <c r="Y534" t="s">
+        <v>314</v>
+      </c>
+      <c r="AB534" t="s">
+        <v>78</v>
+      </c>
+      <c r="AC534" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="535" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A535">
+        <v>386.2</v>
+      </c>
+      <c r="B535" t="s">
+        <v>382</v>
+      </c>
+      <c r="C535" t="s">
+        <v>310</v>
+      </c>
+      <c r="D535" t="s">
+        <v>31</v>
+      </c>
+      <c r="E535" t="s">
+        <v>32</v>
+      </c>
+      <c r="F535" s="3">
+        <v>46023</v>
+      </c>
+      <c r="G535">
+        <v>2026</v>
+      </c>
+      <c r="H535" t="s">
+        <v>518</v>
+      </c>
+      <c r="I535" t="s">
+        <v>518</v>
+      </c>
+      <c r="K535">
+        <f>+K443+K441+K439+K437</f>
+        <v>27575.2022841</v>
+      </c>
+      <c r="L535">
+        <f>+L443+L441+L439+L437</f>
+        <v>27184.360324000001</v>
+      </c>
+      <c r="M535">
+        <f t="shared" ref="M535" si="104">L535/K535</f>
+        <v>0.98582632482354049</v>
+      </c>
+      <c r="N535">
+        <f t="shared" ref="N535:N536" si="105">L535/K535</f>
+        <v>0.98582632482354049</v>
+      </c>
+      <c r="O535" t="s">
+        <v>143</v>
+      </c>
+      <c r="P535" t="s">
+        <v>143</v>
+      </c>
+      <c r="Q535" t="s">
+        <v>489</v>
+      </c>
+      <c r="R535">
+        <v>0</v>
+      </c>
+      <c r="S535">
+        <v>0</v>
+      </c>
+      <c r="T535" t="s">
+        <v>518</v>
+      </c>
+      <c r="U535" t="s">
+        <v>37</v>
+      </c>
+      <c r="V535" t="s">
+        <v>310</v>
+      </c>
+      <c r="W535" t="s">
+        <v>312</v>
+      </c>
+      <c r="X535" t="s">
+        <v>313</v>
+      </c>
+      <c r="Y535" t="s">
+        <v>314</v>
+      </c>
+      <c r="AB535" t="s">
+        <v>78</v>
+      </c>
+      <c r="AC535" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="536" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A536">
+        <v>386.3</v>
+      </c>
+      <c r="B536" t="s">
+        <v>387</v>
+      </c>
+      <c r="C536" t="s">
+        <v>310</v>
+      </c>
+      <c r="D536" t="s">
+        <v>31</v>
+      </c>
+      <c r="E536" t="s">
+        <v>32</v>
+      </c>
+      <c r="F536" s="3">
+        <v>46023</v>
+      </c>
+      <c r="G536">
+        <v>2026</v>
+      </c>
+      <c r="H536" t="s">
+        <v>518</v>
+      </c>
+      <c r="I536" t="s">
+        <v>518</v>
+      </c>
+      <c r="K536">
+        <f>+K451+K449+K447+K445</f>
+        <v>19404.541402700001</v>
+      </c>
+      <c r="L536">
+        <f>+L451+L449+L447+L445</f>
+        <v>18711.499303000001</v>
+      </c>
+      <c r="M536">
+        <f t="shared" ref="M536" si="106">IF(L536/K536&gt;1.3,1.3,L536/K536)</f>
+        <v>0.96428454116397888</v>
+      </c>
+      <c r="N536">
+        <f t="shared" si="105"/>
+        <v>0.96428454116397888</v>
+      </c>
+      <c r="O536" t="s">
+        <v>143</v>
+      </c>
+      <c r="P536" t="s">
+        <v>143</v>
+      </c>
+      <c r="Q536" t="s">
+        <v>492</v>
+      </c>
+      <c r="R536">
+        <v>0</v>
+      </c>
+      <c r="S536">
+        <v>0</v>
+      </c>
+      <c r="T536" t="s">
+        <v>518</v>
+      </c>
+      <c r="U536" t="s">
+        <v>37</v>
+      </c>
+      <c r="V536" t="s">
+        <v>310</v>
+      </c>
+      <c r="W536" t="s">
+        <v>312</v>
+      </c>
+      <c r="X536" t="s">
+        <v>313</v>
+      </c>
+      <c r="Y536" t="s">
+        <v>314</v>
+      </c>
+      <c r="AB536" t="s">
+        <v>78</v>
+      </c>
+      <c r="AC536" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="537" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A537">
+        <v>423</v>
+      </c>
+      <c r="B537" t="s">
+        <v>320</v>
+      </c>
+      <c r="C537" t="s">
+        <v>83</v>
+      </c>
+      <c r="D537" t="s">
+        <v>66</v>
+      </c>
+      <c r="E537" t="s">
+        <v>32</v>
+      </c>
+      <c r="F537" s="3">
+        <v>46023</v>
+      </c>
+      <c r="G537">
+        <v>2026</v>
+      </c>
+      <c r="H537" t="s">
+        <v>518</v>
+      </c>
+      <c r="I537" t="s">
+        <v>518</v>
+      </c>
+      <c r="K537">
+        <v>12</v>
+      </c>
+      <c r="L537">
+        <v>15.1</v>
+      </c>
+      <c r="M537">
+        <f>+L537/K537</f>
+        <v>1.2583333333333333</v>
+      </c>
+      <c r="N537">
+        <f>+L537/K537</f>
+        <v>1.2583333333333333</v>
+      </c>
+      <c r="O537" t="s">
+        <v>245</v>
+      </c>
+      <c r="P537" t="s">
+        <v>245</v>
+      </c>
+      <c r="Q537" t="s">
+        <v>494</v>
+      </c>
+      <c r="R537">
+        <v>1</v>
+      </c>
+      <c r="S537">
+        <v>1</v>
+      </c>
+      <c r="T537" t="s">
+        <v>518</v>
+      </c>
+      <c r="U537" t="s">
+        <v>37</v>
+      </c>
+      <c r="V537" t="s">
+        <v>83</v>
+      </c>
+      <c r="W537" t="s">
+        <v>38</v>
+      </c>
+      <c r="X537" t="s">
+        <v>39</v>
+      </c>
+      <c r="Y537" t="s">
+        <v>322</v>
+      </c>
+      <c r="Z537" t="s">
+        <v>274</v>
+      </c>
+      <c r="AA537" t="s">
+        <v>275</v>
+      </c>
+      <c r="AB537" t="s">
+        <v>43</v>
+      </c>
+      <c r="AC537" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="538" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A538">
+        <v>424</v>
+      </c>
+      <c r="B538" t="s">
+        <v>325</v>
+      </c>
+      <c r="C538" t="s">
+        <v>83</v>
+      </c>
+      <c r="D538" t="s">
+        <v>66</v>
+      </c>
+      <c r="E538" t="s">
+        <v>32</v>
+      </c>
+      <c r="F538" s="3">
+        <v>46023</v>
+      </c>
+      <c r="G538">
+        <v>2026</v>
+      </c>
+      <c r="H538" t="s">
+        <v>518</v>
+      </c>
+      <c r="I538" t="s">
+        <v>518</v>
+      </c>
+      <c r="K538">
+        <v>9</v>
+      </c>
+      <c r="L538">
+        <v>11</v>
+      </c>
+      <c r="M538">
+        <f>+L538/K538</f>
+        <v>1.2222222222222223</v>
+      </c>
+      <c r="N538">
+        <f>+L538/K538</f>
+        <v>1.2222222222222223</v>
+      </c>
+      <c r="O538" t="s">
+        <v>35</v>
+      </c>
+      <c r="P538" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q538" t="s">
+        <v>495</v>
+      </c>
+      <c r="R538">
+        <v>0</v>
+      </c>
+      <c r="S538">
+        <v>0</v>
+      </c>
+      <c r="T538" t="s">
+        <v>518</v>
+      </c>
+      <c r="U538" t="s">
+        <v>37</v>
+      </c>
+      <c r="V538" t="s">
+        <v>83</v>
+      </c>
+      <c r="W538" t="s">
+        <v>38</v>
+      </c>
+      <c r="X538" t="s">
+        <v>39</v>
+      </c>
+      <c r="Y538" t="s">
+        <v>322</v>
+      </c>
+      <c r="Z538" t="s">
+        <v>274</v>
+      </c>
+      <c r="AA538" t="s">
+        <v>275</v>
+      </c>
+      <c r="AB538" t="s">
+        <v>43</v>
+      </c>
+      <c r="AC538" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="539" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A539">
+        <v>466</v>
+      </c>
+      <c r="B539" t="s">
+        <v>341</v>
+      </c>
+      <c r="C539" t="s">
+        <v>30</v>
+      </c>
+      <c r="D539" t="s">
+        <v>31</v>
+      </c>
+      <c r="E539" t="s">
+        <v>32</v>
+      </c>
+      <c r="F539" s="3">
+        <v>46023</v>
+      </c>
+      <c r="G539">
+        <v>2026</v>
+      </c>
+      <c r="H539" t="s">
+        <v>518</v>
+      </c>
+      <c r="I539" t="s">
+        <v>518</v>
+      </c>
+      <c r="K539">
+        <v>55</v>
+      </c>
+      <c r="L539">
+        <v>58.6</v>
+      </c>
+      <c r="M539">
+        <f t="shared" ref="M539" si="107">+L539/K539</f>
+        <v>1.0654545454545454</v>
+      </c>
+      <c r="N539">
+        <f>+L539/K539</f>
+        <v>1.0654545454545454</v>
+      </c>
+      <c r="O539" t="s">
+        <v>35</v>
+      </c>
+      <c r="P539" t="s">
+        <v>245</v>
+      </c>
+      <c r="Q539" t="s">
+        <v>487</v>
+      </c>
+      <c r="R539">
+        <v>1</v>
+      </c>
+      <c r="S539">
+        <v>1</v>
+      </c>
+      <c r="T539" t="s">
+        <v>518</v>
+      </c>
+      <c r="U539" t="s">
+        <v>37</v>
+      </c>
+      <c r="V539" t="s">
+        <v>342</v>
+      </c>
+      <c r="W539" t="s">
+        <v>112</v>
+      </c>
+      <c r="X539" t="s">
+        <v>113</v>
+      </c>
+      <c r="Y539" t="s">
+        <v>114</v>
+      </c>
+      <c r="Z539" t="s">
+        <v>41</v>
+      </c>
+      <c r="AA539" t="s">
+        <v>102</v>
+      </c>
+      <c r="AB539" t="s">
+        <v>43</v>
+      </c>
+      <c r="AC539" t="s">
         <v>66</v>
       </c>
     </row>

</xml_diff>